<commit_message>
added 38 ILMN-DV callsets
</commit_message>
<xml_diff>
--- a/config/analyses_44_template.xlsx
+++ b/config/analyses_44_template.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,19 +8,30 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jmcdani/Documents/GiaB/Benchmarking/assembly-benchmark-development/giab-asm-bench-whole-genome/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{FB880233-116E-0B40-BEE4-9B1643751321}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAF7AD50-8B9A-9E4A-84AC-CB104803A061}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4300" yWindow="2700" windowWidth="27640" windowHeight="16940"/>
+    <workbookView xWindow="-34560" yWindow="-220" windowWidth="27640" windowHeight="16940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="analyses_44" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1018" uniqueCount="78">
   <si>
     <t>eval_id</t>
   </si>
@@ -254,270 +265,12 @@
   </si>
   <si>
     <t>HG03579</t>
-  </si>
-  <si>
-    <t>GRCh39</t>
-  </si>
-  <si>
-    <t>-z200000,10001</t>
-  </si>
-  <si>
-    <t>GRCh40</t>
-  </si>
-  <si>
-    <t>-z200000,10002</t>
-  </si>
-  <si>
-    <t>GRCh41</t>
-  </si>
-  <si>
-    <t>-z200000,10003</t>
-  </si>
-  <si>
-    <t>GRCh42</t>
-  </si>
-  <si>
-    <t>-z200000,10004</t>
-  </si>
-  <si>
-    <t>GRCh43</t>
-  </si>
-  <si>
-    <t>-z200000,10005</t>
-  </si>
-  <si>
-    <t>GRCh44</t>
-  </si>
-  <si>
-    <t>-z200000,10006</t>
-  </si>
-  <si>
-    <t>GRCh45</t>
-  </si>
-  <si>
-    <t>-z200000,10007</t>
-  </si>
-  <si>
-    <t>GRCh46</t>
-  </si>
-  <si>
-    <t>-z200000,10008</t>
-  </si>
-  <si>
-    <t>GRCh47</t>
-  </si>
-  <si>
-    <t>-z200000,10009</t>
-  </si>
-  <si>
-    <t>GRCh48</t>
-  </si>
-  <si>
-    <t>-z200000,10010</t>
-  </si>
-  <si>
-    <t>GRCh49</t>
-  </si>
-  <si>
-    <t>-z200000,10011</t>
-  </si>
-  <si>
-    <t>GRCh50</t>
-  </si>
-  <si>
-    <t>-z200000,10012</t>
-  </si>
-  <si>
-    <t>GRCh51</t>
-  </si>
-  <si>
-    <t>-z200000,10013</t>
-  </si>
-  <si>
-    <t>GRCh52</t>
-  </si>
-  <si>
-    <t>-z200000,10014</t>
-  </si>
-  <si>
-    <t>GRCh53</t>
-  </si>
-  <si>
-    <t>-z200000,10015</t>
-  </si>
-  <si>
-    <t>GRCh54</t>
-  </si>
-  <si>
-    <t>-z200000,10016</t>
-  </si>
-  <si>
-    <t>GRCh55</t>
-  </si>
-  <si>
-    <t>-z200000,10017</t>
-  </si>
-  <si>
-    <t>GRCh56</t>
-  </si>
-  <si>
-    <t>-z200000,10018</t>
-  </si>
-  <si>
-    <t>GRCh57</t>
-  </si>
-  <si>
-    <t>-z200000,10019</t>
-  </si>
-  <si>
-    <t>GRCh58</t>
-  </si>
-  <si>
-    <t>-z200000,10020</t>
-  </si>
-  <si>
-    <t>GRCh59</t>
-  </si>
-  <si>
-    <t>-z200000,10021</t>
-  </si>
-  <si>
-    <t>GRCh60</t>
-  </si>
-  <si>
-    <t>-z200000,10022</t>
-  </si>
-  <si>
-    <t>GRCh61</t>
-  </si>
-  <si>
-    <t>-z200000,10023</t>
-  </si>
-  <si>
-    <t>GRCh62</t>
-  </si>
-  <si>
-    <t>-z200000,10024</t>
-  </si>
-  <si>
-    <t>GRCh63</t>
-  </si>
-  <si>
-    <t>-z200000,10025</t>
-  </si>
-  <si>
-    <t>GRCh64</t>
-  </si>
-  <si>
-    <t>-z200000,10026</t>
-  </si>
-  <si>
-    <t>GRCh65</t>
-  </si>
-  <si>
-    <t>-z200000,10027</t>
-  </si>
-  <si>
-    <t>GRCh66</t>
-  </si>
-  <si>
-    <t>-z200000,10028</t>
-  </si>
-  <si>
-    <t>GRCh67</t>
-  </si>
-  <si>
-    <t>-z200000,10029</t>
-  </si>
-  <si>
-    <t>GRCh68</t>
-  </si>
-  <si>
-    <t>-z200000,10030</t>
-  </si>
-  <si>
-    <t>GRCh69</t>
-  </si>
-  <si>
-    <t>-z200000,10031</t>
-  </si>
-  <si>
-    <t>GRCh70</t>
-  </si>
-  <si>
-    <t>-z200000,10032</t>
-  </si>
-  <si>
-    <t>GRCh71</t>
-  </si>
-  <si>
-    <t>-z200000,10033</t>
-  </si>
-  <si>
-    <t>GRCh72</t>
-  </si>
-  <si>
-    <t>-z200000,10034</t>
-  </si>
-  <si>
-    <t>GRCh73</t>
-  </si>
-  <si>
-    <t>-z200000,10035</t>
-  </si>
-  <si>
-    <t>GRCh74</t>
-  </si>
-  <si>
-    <t>-z200000,10036</t>
-  </si>
-  <si>
-    <t>GRCh75</t>
-  </si>
-  <si>
-    <t>-z200000,10037</t>
-  </si>
-  <si>
-    <t>GRCh76</t>
-  </si>
-  <si>
-    <t>-z200000,10038</t>
-  </si>
-  <si>
-    <t>GRCh77</t>
-  </si>
-  <si>
-    <t>-z200000,10039</t>
-  </si>
-  <si>
-    <t>GRCh78</t>
-  </si>
-  <si>
-    <t>-z200000,10040</t>
-  </si>
-  <si>
-    <t>GRCh79</t>
-  </si>
-  <si>
-    <t>-z200000,10041</t>
-  </si>
-  <si>
-    <t>GRCh80</t>
-  </si>
-  <si>
-    <t>-z200000,10042</t>
-  </si>
-  <si>
-    <t>GRCh81</t>
-  </si>
-  <si>
-    <t>-z200000,10043</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -660,7 +413,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -840,6 +593,12 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -1001,8 +760,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1357,11 +1117,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S46"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:S84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="200" workbookViewId="0">
-      <selection activeCell="S47" sqref="S47"/>
+    <sheetView tabSelected="1" topLeftCell="O67" zoomScale="200" workbookViewId="0">
+      <selection activeCell="K83" sqref="K83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1521,6 +1281,9 @@
         <f>CONCATENATE("GRCh38_HPRC-",A3,"_dipz2k")</f>
         <v>GRCh38_HPRC-HG00733_dipz2k</v>
       </c>
+      <c r="K3" t="s">
+        <v>24</v>
+      </c>
       <c r="L3" t="s">
         <v>25</v>
       </c>
@@ -1582,6 +1345,9 @@
         <f t="shared" ref="J4:J45" si="3">CONCATENATE("GRCh38_HPRC-",A4,"_dipz2k")</f>
         <v>GRCh38_HPRC-HG01109_dipz2k</v>
       </c>
+      <c r="K4" t="s">
+        <v>24</v>
+      </c>
       <c r="L4" t="s">
         <v>25</v>
       </c>
@@ -1596,7 +1362,7 @@
         <v>HPRC-HG01109</v>
       </c>
       <c r="P4" t="s">
-        <v>78</v>
+        <v>29</v>
       </c>
       <c r="Q4" t="s">
         <v>30</v>
@@ -1605,7 +1371,7 @@
         <v>31</v>
       </c>
       <c r="S4" t="s">
-        <v>79</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.2">
@@ -1643,6 +1409,9 @@
         <f t="shared" si="3"/>
         <v>GRCh38_HPRC-HG01243_dipz2k</v>
       </c>
+      <c r="K5" t="s">
+        <v>24</v>
+      </c>
       <c r="L5" t="s">
         <v>25</v>
       </c>
@@ -1657,7 +1426,7 @@
         <v>HPRC-HG01243</v>
       </c>
       <c r="P5" t="s">
-        <v>80</v>
+        <v>29</v>
       </c>
       <c r="Q5" t="s">
         <v>30</v>
@@ -1666,7 +1435,7 @@
         <v>31</v>
       </c>
       <c r="S5" t="s">
-        <v>81</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.2">
@@ -1704,6 +1473,9 @@
         <f t="shared" si="3"/>
         <v>GRCh38_HPRC-HG02055_dipz2k</v>
       </c>
+      <c r="K6" t="s">
+        <v>24</v>
+      </c>
       <c r="L6" t="s">
         <v>25</v>
       </c>
@@ -1718,7 +1490,7 @@
         <v>HPRC-HG02055</v>
       </c>
       <c r="P6" t="s">
-        <v>82</v>
+        <v>29</v>
       </c>
       <c r="Q6" t="s">
         <v>30</v>
@@ -1727,7 +1499,7 @@
         <v>31</v>
       </c>
       <c r="S6" t="s">
-        <v>83</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.2">
@@ -1765,6 +1537,9 @@
         <f t="shared" si="3"/>
         <v>GRCh38_HPRC-HG02080_dipz2k</v>
       </c>
+      <c r="K7" t="s">
+        <v>24</v>
+      </c>
       <c r="L7" t="s">
         <v>25</v>
       </c>
@@ -1779,7 +1554,7 @@
         <v>HPRC-HG02080</v>
       </c>
       <c r="P7" t="s">
-        <v>84</v>
+        <v>29</v>
       </c>
       <c r="Q7" t="s">
         <v>30</v>
@@ -1788,7 +1563,7 @@
         <v>31</v>
       </c>
       <c r="S7" t="s">
-        <v>85</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.2">
@@ -1826,6 +1601,9 @@
         <f t="shared" si="3"/>
         <v>GRCh38_HPRC-HG02109_dipz2k</v>
       </c>
+      <c r="K8" t="s">
+        <v>24</v>
+      </c>
       <c r="L8" t="s">
         <v>25</v>
       </c>
@@ -1840,7 +1618,7 @@
         <v>HPRC-HG02109</v>
       </c>
       <c r="P8" t="s">
-        <v>86</v>
+        <v>29</v>
       </c>
       <c r="Q8" t="s">
         <v>30</v>
@@ -1849,7 +1627,7 @@
         <v>31</v>
       </c>
       <c r="S8" t="s">
-        <v>87</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.2">
@@ -1887,6 +1665,9 @@
         <f t="shared" si="3"/>
         <v>GRCh38_HPRC-HG02145_dipz2k</v>
       </c>
+      <c r="K9" t="s">
+        <v>24</v>
+      </c>
       <c r="L9" t="s">
         <v>25</v>
       </c>
@@ -1901,7 +1682,7 @@
         <v>HPRC-HG02145</v>
       </c>
       <c r="P9" t="s">
-        <v>88</v>
+        <v>29</v>
       </c>
       <c r="Q9" t="s">
         <v>30</v>
@@ -1910,7 +1691,7 @@
         <v>31</v>
       </c>
       <c r="S9" t="s">
-        <v>89</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.2">
@@ -1948,6 +1729,9 @@
         <f t="shared" si="3"/>
         <v>GRCh38_HPRC-HG02723_dipz2k</v>
       </c>
+      <c r="K10" t="s">
+        <v>24</v>
+      </c>
       <c r="L10" t="s">
         <v>25</v>
       </c>
@@ -1962,7 +1746,7 @@
         <v>HPRC-HG02723</v>
       </c>
       <c r="P10" t="s">
-        <v>90</v>
+        <v>29</v>
       </c>
       <c r="Q10" t="s">
         <v>30</v>
@@ -1971,7 +1755,7 @@
         <v>31</v>
       </c>
       <c r="S10" t="s">
-        <v>91</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.2">
@@ -2009,6 +1793,9 @@
         <f t="shared" si="3"/>
         <v>GRCh38_HPRC-HG02818_dipz2k</v>
       </c>
+      <c r="K11" t="s">
+        <v>24</v>
+      </c>
       <c r="L11" t="s">
         <v>25</v>
       </c>
@@ -2023,7 +1810,7 @@
         <v>HPRC-HG02818</v>
       </c>
       <c r="P11" t="s">
-        <v>92</v>
+        <v>29</v>
       </c>
       <c r="Q11" t="s">
         <v>30</v>
@@ -2032,7 +1819,7 @@
         <v>31</v>
       </c>
       <c r="S11" t="s">
-        <v>93</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.2">
@@ -2070,6 +1857,9 @@
         <f t="shared" si="3"/>
         <v>GRCh38_HPRC-HG03098_dipz2k</v>
       </c>
+      <c r="K12" t="s">
+        <v>24</v>
+      </c>
       <c r="L12" t="s">
         <v>25</v>
       </c>
@@ -2084,7 +1874,7 @@
         <v>HPRC-HG03098</v>
       </c>
       <c r="P12" t="s">
-        <v>94</v>
+        <v>29</v>
       </c>
       <c r="Q12" t="s">
         <v>30</v>
@@ -2093,7 +1883,7 @@
         <v>31</v>
       </c>
       <c r="S12" t="s">
-        <v>95</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.2">
@@ -2131,6 +1921,9 @@
         <f t="shared" si="3"/>
         <v>GRCh38_HPRC-HG03486_dipz2k</v>
       </c>
+      <c r="K13" t="s">
+        <v>24</v>
+      </c>
       <c r="L13" t="s">
         <v>25</v>
       </c>
@@ -2145,7 +1938,7 @@
         <v>HPRC-HG03486</v>
       </c>
       <c r="P13" t="s">
-        <v>96</v>
+        <v>29</v>
       </c>
       <c r="Q13" t="s">
         <v>30</v>
@@ -2154,7 +1947,7 @@
         <v>31</v>
       </c>
       <c r="S13" t="s">
-        <v>97</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.2">
@@ -2192,6 +1985,9 @@
         <f t="shared" si="3"/>
         <v>GRCh38_HPRC-HG03492_dipz2k</v>
       </c>
+      <c r="K14" t="s">
+        <v>24</v>
+      </c>
       <c r="L14" t="s">
         <v>25</v>
       </c>
@@ -2206,7 +2002,7 @@
         <v>HPRC-HG03492</v>
       </c>
       <c r="P14" t="s">
-        <v>98</v>
+        <v>29</v>
       </c>
       <c r="Q14" t="s">
         <v>30</v>
@@ -2215,7 +2011,7 @@
         <v>31</v>
       </c>
       <c r="S14" t="s">
-        <v>99</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.2">
@@ -2253,6 +2049,9 @@
         <f t="shared" si="3"/>
         <v>GRCh38_HPRC-NA18906_dipz2k</v>
       </c>
+      <c r="K15" t="s">
+        <v>24</v>
+      </c>
       <c r="L15" t="s">
         <v>25</v>
       </c>
@@ -2267,7 +2066,7 @@
         <v>HPRC-NA18906</v>
       </c>
       <c r="P15" t="s">
-        <v>100</v>
+        <v>29</v>
       </c>
       <c r="Q15" t="s">
         <v>30</v>
@@ -2276,7 +2075,7 @@
         <v>31</v>
       </c>
       <c r="S15" t="s">
-        <v>101</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.2">
@@ -2314,6 +2113,9 @@
         <f t="shared" si="3"/>
         <v>GRCh38_HPRC-NA20129_dipz2k</v>
       </c>
+      <c r="K16" t="s">
+        <v>24</v>
+      </c>
       <c r="L16" t="s">
         <v>25</v>
       </c>
@@ -2328,7 +2130,7 @@
         <v>HPRC-NA20129</v>
       </c>
       <c r="P16" t="s">
-        <v>102</v>
+        <v>29</v>
       </c>
       <c r="Q16" t="s">
         <v>30</v>
@@ -2337,7 +2139,7 @@
         <v>31</v>
       </c>
       <c r="S16" t="s">
-        <v>103</v>
+        <v>32</v>
       </c>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.2">
@@ -2375,6 +2177,9 @@
         <f t="shared" si="3"/>
         <v>GRCh38_HPRC-NA21309_dipz2k</v>
       </c>
+      <c r="K17" t="s">
+        <v>24</v>
+      </c>
       <c r="L17" t="s">
         <v>25</v>
       </c>
@@ -2389,7 +2194,7 @@
         <v>HPRC-NA21309</v>
       </c>
       <c r="P17" t="s">
-        <v>104</v>
+        <v>29</v>
       </c>
       <c r="Q17" t="s">
         <v>30</v>
@@ -2398,7 +2203,7 @@
         <v>31</v>
       </c>
       <c r="S17" t="s">
-        <v>105</v>
+        <v>32</v>
       </c>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.2">
@@ -2436,6 +2241,9 @@
         <f t="shared" si="3"/>
         <v>GRCh38_HPRC-HG00438_dipz2k</v>
       </c>
+      <c r="K18" t="s">
+        <v>24</v>
+      </c>
       <c r="L18" t="s">
         <v>25</v>
       </c>
@@ -2450,7 +2258,7 @@
         <v>HPRC-HG00438</v>
       </c>
       <c r="P18" t="s">
-        <v>106</v>
+        <v>29</v>
       </c>
       <c r="Q18" t="s">
         <v>30</v>
@@ -2459,7 +2267,7 @@
         <v>31</v>
       </c>
       <c r="S18" t="s">
-        <v>107</v>
+        <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.2">
@@ -2497,6 +2305,9 @@
         <f t="shared" si="3"/>
         <v>GRCh38_HPRC-HG00621_dipz2k</v>
       </c>
+      <c r="K19" t="s">
+        <v>24</v>
+      </c>
       <c r="L19" t="s">
         <v>25</v>
       </c>
@@ -2511,7 +2322,7 @@
         <v>HPRC-HG00621</v>
       </c>
       <c r="P19" t="s">
-        <v>108</v>
+        <v>29</v>
       </c>
       <c r="Q19" t="s">
         <v>30</v>
@@ -2520,7 +2331,7 @@
         <v>31</v>
       </c>
       <c r="S19" t="s">
-        <v>109</v>
+        <v>32</v>
       </c>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.2">
@@ -2558,6 +2369,9 @@
         <f t="shared" si="3"/>
         <v>GRCh38_HPRC-HG00673_dipz2k</v>
       </c>
+      <c r="K20" t="s">
+        <v>24</v>
+      </c>
       <c r="L20" t="s">
         <v>25</v>
       </c>
@@ -2572,7 +2386,7 @@
         <v>HPRC-HG00673</v>
       </c>
       <c r="P20" t="s">
-        <v>110</v>
+        <v>29</v>
       </c>
       <c r="Q20" t="s">
         <v>30</v>
@@ -2581,7 +2395,7 @@
         <v>31</v>
       </c>
       <c r="S20" t="s">
-        <v>111</v>
+        <v>32</v>
       </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.2">
@@ -2619,6 +2433,9 @@
         <f t="shared" si="3"/>
         <v>GRCh38_HPRC-HG00735_dipz2k</v>
       </c>
+      <c r="K21" t="s">
+        <v>24</v>
+      </c>
       <c r="L21" t="s">
         <v>25</v>
       </c>
@@ -2633,7 +2450,7 @@
         <v>HPRC-HG00735</v>
       </c>
       <c r="P21" t="s">
-        <v>112</v>
+        <v>29</v>
       </c>
       <c r="Q21" t="s">
         <v>30</v>
@@ -2642,7 +2459,7 @@
         <v>31</v>
       </c>
       <c r="S21" t="s">
-        <v>113</v>
+        <v>32</v>
       </c>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.2">
@@ -2680,6 +2497,9 @@
         <f t="shared" si="3"/>
         <v>GRCh38_HPRC-HG00741_dipz2k</v>
       </c>
+      <c r="K22" t="s">
+        <v>24</v>
+      </c>
       <c r="L22" t="s">
         <v>25</v>
       </c>
@@ -2694,7 +2514,7 @@
         <v>HPRC-HG00741</v>
       </c>
       <c r="P22" t="s">
-        <v>114</v>
+        <v>29</v>
       </c>
       <c r="Q22" t="s">
         <v>30</v>
@@ -2703,7 +2523,7 @@
         <v>31</v>
       </c>
       <c r="S22" t="s">
-        <v>115</v>
+        <v>32</v>
       </c>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.2">
@@ -2741,6 +2561,9 @@
         <f t="shared" si="3"/>
         <v>GRCh38_HPRC-HG01071_dipz2k</v>
       </c>
+      <c r="K23" t="s">
+        <v>24</v>
+      </c>
       <c r="L23" t="s">
         <v>25</v>
       </c>
@@ -2755,7 +2578,7 @@
         <v>HPRC-HG01071</v>
       </c>
       <c r="P23" t="s">
-        <v>116</v>
+        <v>29</v>
       </c>
       <c r="Q23" t="s">
         <v>30</v>
@@ -2764,7 +2587,7 @@
         <v>31</v>
       </c>
       <c r="S23" t="s">
-        <v>117</v>
+        <v>32</v>
       </c>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.2">
@@ -2802,6 +2625,9 @@
         <f t="shared" si="3"/>
         <v>GRCh38_HPRC-HG01106_dipz2k</v>
       </c>
+      <c r="K24" t="s">
+        <v>24</v>
+      </c>
       <c r="L24" t="s">
         <v>25</v>
       </c>
@@ -2816,7 +2642,7 @@
         <v>HPRC-HG01106</v>
       </c>
       <c r="P24" t="s">
-        <v>118</v>
+        <v>29</v>
       </c>
       <c r="Q24" t="s">
         <v>30</v>
@@ -2825,7 +2651,7 @@
         <v>31</v>
       </c>
       <c r="S24" t="s">
-        <v>119</v>
+        <v>32</v>
       </c>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.2">
@@ -2863,6 +2689,9 @@
         <f t="shared" si="3"/>
         <v>GRCh38_HPRC-HG01123_dipz2k</v>
       </c>
+      <c r="K25" t="s">
+        <v>24</v>
+      </c>
       <c r="L25" t="s">
         <v>25</v>
       </c>
@@ -2877,7 +2706,7 @@
         <v>HPRC-HG01123</v>
       </c>
       <c r="P25" t="s">
-        <v>120</v>
+        <v>29</v>
       </c>
       <c r="Q25" t="s">
         <v>30</v>
@@ -2886,7 +2715,7 @@
         <v>31</v>
       </c>
       <c r="S25" t="s">
-        <v>121</v>
+        <v>32</v>
       </c>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.2">
@@ -2924,6 +2753,9 @@
         <f t="shared" si="3"/>
         <v>GRCh38_HPRC-HG01175_dipz2k</v>
       </c>
+      <c r="K26" t="s">
+        <v>24</v>
+      </c>
       <c r="L26" t="s">
         <v>25</v>
       </c>
@@ -2938,7 +2770,7 @@
         <v>HPRC-HG01175</v>
       </c>
       <c r="P26" t="s">
-        <v>122</v>
+        <v>29</v>
       </c>
       <c r="Q26" t="s">
         <v>30</v>
@@ -2947,7 +2779,7 @@
         <v>31</v>
       </c>
       <c r="S26" t="s">
-        <v>123</v>
+        <v>32</v>
       </c>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.2">
@@ -2985,6 +2817,9 @@
         <f t="shared" si="3"/>
         <v>GRCh38_HPRC-HG01258_dipz2k</v>
       </c>
+      <c r="K27" t="s">
+        <v>24</v>
+      </c>
       <c r="L27" t="s">
         <v>25</v>
       </c>
@@ -2999,7 +2834,7 @@
         <v>HPRC-HG01258</v>
       </c>
       <c r="P27" t="s">
-        <v>124</v>
+        <v>29</v>
       </c>
       <c r="Q27" t="s">
         <v>30</v>
@@ -3008,7 +2843,7 @@
         <v>31</v>
       </c>
       <c r="S27" t="s">
-        <v>125</v>
+        <v>32</v>
       </c>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.2">
@@ -3046,6 +2881,9 @@
         <f t="shared" si="3"/>
         <v>GRCh38_HPRC-HG01358_dipz2k</v>
       </c>
+      <c r="K28" t="s">
+        <v>24</v>
+      </c>
       <c r="L28" t="s">
         <v>25</v>
       </c>
@@ -3060,7 +2898,7 @@
         <v>HPRC-HG01358</v>
       </c>
       <c r="P28" t="s">
-        <v>126</v>
+        <v>29</v>
       </c>
       <c r="Q28" t="s">
         <v>30</v>
@@ -3069,7 +2907,7 @@
         <v>31</v>
       </c>
       <c r="S28" t="s">
-        <v>127</v>
+        <v>32</v>
       </c>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.2">
@@ -3107,6 +2945,9 @@
         <f t="shared" si="3"/>
         <v>GRCh38_HPRC-HG01361_dipz2k</v>
       </c>
+      <c r="K29" t="s">
+        <v>24</v>
+      </c>
       <c r="L29" t="s">
         <v>25</v>
       </c>
@@ -3121,7 +2962,7 @@
         <v>HPRC-HG01361</v>
       </c>
       <c r="P29" t="s">
-        <v>128</v>
+        <v>29</v>
       </c>
       <c r="Q29" t="s">
         <v>30</v>
@@ -3130,7 +2971,7 @@
         <v>31</v>
       </c>
       <c r="S29" t="s">
-        <v>129</v>
+        <v>32</v>
       </c>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.2">
@@ -3168,6 +3009,9 @@
         <f t="shared" si="3"/>
         <v>GRCh38_HPRC-HG01891_dipz2k</v>
       </c>
+      <c r="K30" t="s">
+        <v>24</v>
+      </c>
       <c r="L30" t="s">
         <v>25</v>
       </c>
@@ -3182,7 +3026,7 @@
         <v>HPRC-HG01891</v>
       </c>
       <c r="P30" t="s">
-        <v>130</v>
+        <v>29</v>
       </c>
       <c r="Q30" t="s">
         <v>30</v>
@@ -3191,7 +3035,7 @@
         <v>31</v>
       </c>
       <c r="S30" t="s">
-        <v>131</v>
+        <v>32</v>
       </c>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.2">
@@ -3229,6 +3073,9 @@
         <f t="shared" si="3"/>
         <v>GRCh38_HPRC-HG01928_dipz2k</v>
       </c>
+      <c r="K31" t="s">
+        <v>24</v>
+      </c>
       <c r="L31" t="s">
         <v>25</v>
       </c>
@@ -3243,7 +3090,7 @@
         <v>HPRC-HG01928</v>
       </c>
       <c r="P31" t="s">
-        <v>132</v>
+        <v>29</v>
       </c>
       <c r="Q31" t="s">
         <v>30</v>
@@ -3252,7 +3099,7 @@
         <v>31</v>
       </c>
       <c r="S31" t="s">
-        <v>133</v>
+        <v>32</v>
       </c>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.2">
@@ -3290,6 +3137,9 @@
         <f t="shared" si="3"/>
         <v>GRCh38_HPRC-HG01952_dipz2k</v>
       </c>
+      <c r="K32" t="s">
+        <v>24</v>
+      </c>
       <c r="L32" t="s">
         <v>25</v>
       </c>
@@ -3304,7 +3154,7 @@
         <v>HPRC-HG01952</v>
       </c>
       <c r="P32" t="s">
-        <v>134</v>
+        <v>29</v>
       </c>
       <c r="Q32" t="s">
         <v>30</v>
@@ -3313,7 +3163,7 @@
         <v>31</v>
       </c>
       <c r="S32" t="s">
-        <v>135</v>
+        <v>32</v>
       </c>
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.2">
@@ -3351,6 +3201,9 @@
         <f t="shared" si="3"/>
         <v>GRCh38_HPRC-HG01978_dipz2k</v>
       </c>
+      <c r="K33" t="s">
+        <v>24</v>
+      </c>
       <c r="L33" t="s">
         <v>25</v>
       </c>
@@ -3365,7 +3218,7 @@
         <v>HPRC-HG01978</v>
       </c>
       <c r="P33" t="s">
-        <v>136</v>
+        <v>29</v>
       </c>
       <c r="Q33" t="s">
         <v>30</v>
@@ -3374,7 +3227,7 @@
         <v>31</v>
       </c>
       <c r="S33" t="s">
-        <v>137</v>
+        <v>32</v>
       </c>
     </row>
     <row r="34" spans="1:19" x14ac:dyDescent="0.2">
@@ -3412,6 +3265,9 @@
         <f t="shared" si="3"/>
         <v>GRCh38_HPRC-HG02148_dipz2k</v>
       </c>
+      <c r="K34" t="s">
+        <v>24</v>
+      </c>
       <c r="L34" t="s">
         <v>25</v>
       </c>
@@ -3426,7 +3282,7 @@
         <v>HPRC-HG02148</v>
       </c>
       <c r="P34" t="s">
-        <v>138</v>
+        <v>29</v>
       </c>
       <c r="Q34" t="s">
         <v>30</v>
@@ -3435,7 +3291,7 @@
         <v>31</v>
       </c>
       <c r="S34" t="s">
-        <v>139</v>
+        <v>32</v>
       </c>
     </row>
     <row r="35" spans="1:19" x14ac:dyDescent="0.2">
@@ -3473,6 +3329,9 @@
         <f t="shared" si="3"/>
         <v>GRCh38_HPRC-HG02257_dipz2k</v>
       </c>
+      <c r="K35" t="s">
+        <v>24</v>
+      </c>
       <c r="L35" t="s">
         <v>25</v>
       </c>
@@ -3487,7 +3346,7 @@
         <v>HPRC-HG02257</v>
       </c>
       <c r="P35" t="s">
-        <v>140</v>
+        <v>29</v>
       </c>
       <c r="Q35" t="s">
         <v>30</v>
@@ -3496,7 +3355,7 @@
         <v>31</v>
       </c>
       <c r="S35" t="s">
-        <v>141</v>
+        <v>32</v>
       </c>
     </row>
     <row r="36" spans="1:19" x14ac:dyDescent="0.2">
@@ -3534,6 +3393,9 @@
         <f t="shared" si="3"/>
         <v>GRCh38_HPRC-HG02486_dipz2k</v>
       </c>
+      <c r="K36" t="s">
+        <v>24</v>
+      </c>
       <c r="L36" t="s">
         <v>25</v>
       </c>
@@ -3548,7 +3410,7 @@
         <v>HPRC-HG02486</v>
       </c>
       <c r="P36" t="s">
-        <v>142</v>
+        <v>29</v>
       </c>
       <c r="Q36" t="s">
         <v>30</v>
@@ -3557,7 +3419,7 @@
         <v>31</v>
       </c>
       <c r="S36" t="s">
-        <v>143</v>
+        <v>32</v>
       </c>
     </row>
     <row r="37" spans="1:19" x14ac:dyDescent="0.2">
@@ -3595,6 +3457,9 @@
         <f t="shared" si="3"/>
         <v>GRCh38_HPRC-HG02559_dipz2k</v>
       </c>
+      <c r="K37" t="s">
+        <v>24</v>
+      </c>
       <c r="L37" t="s">
         <v>25</v>
       </c>
@@ -3609,7 +3474,7 @@
         <v>HPRC-HG02559</v>
       </c>
       <c r="P37" t="s">
-        <v>144</v>
+        <v>29</v>
       </c>
       <c r="Q37" t="s">
         <v>30</v>
@@ -3618,7 +3483,7 @@
         <v>31</v>
       </c>
       <c r="S37" t="s">
-        <v>145</v>
+        <v>32</v>
       </c>
     </row>
     <row r="38" spans="1:19" x14ac:dyDescent="0.2">
@@ -3656,6 +3521,9 @@
         <f t="shared" si="3"/>
         <v>GRCh38_HPRC-HG02572_dipz2k</v>
       </c>
+      <c r="K38" t="s">
+        <v>24</v>
+      </c>
       <c r="L38" t="s">
         <v>25</v>
       </c>
@@ -3670,7 +3538,7 @@
         <v>HPRC-HG02572</v>
       </c>
       <c r="P38" t="s">
-        <v>146</v>
+        <v>29</v>
       </c>
       <c r="Q38" t="s">
         <v>30</v>
@@ -3679,7 +3547,7 @@
         <v>31</v>
       </c>
       <c r="S38" t="s">
-        <v>147</v>
+        <v>32</v>
       </c>
     </row>
     <row r="39" spans="1:19" x14ac:dyDescent="0.2">
@@ -3717,6 +3585,9 @@
         <f t="shared" si="3"/>
         <v>GRCh38_HPRC-HG02622_dipz2k</v>
       </c>
+      <c r="K39" t="s">
+        <v>24</v>
+      </c>
       <c r="L39" t="s">
         <v>25</v>
       </c>
@@ -3731,7 +3602,7 @@
         <v>HPRC-HG02622</v>
       </c>
       <c r="P39" t="s">
-        <v>148</v>
+        <v>29</v>
       </c>
       <c r="Q39" t="s">
         <v>30</v>
@@ -3740,7 +3611,7 @@
         <v>31</v>
       </c>
       <c r="S39" t="s">
-        <v>149</v>
+        <v>32</v>
       </c>
     </row>
     <row r="40" spans="1:19" x14ac:dyDescent="0.2">
@@ -3778,6 +3649,9 @@
         <f t="shared" si="3"/>
         <v>GRCh38_HPRC-HG02630_dipz2k</v>
       </c>
+      <c r="K40" t="s">
+        <v>24</v>
+      </c>
       <c r="L40" t="s">
         <v>25</v>
       </c>
@@ -3792,7 +3666,7 @@
         <v>HPRC-HG02630</v>
       </c>
       <c r="P40" t="s">
-        <v>150</v>
+        <v>29</v>
       </c>
       <c r="Q40" t="s">
         <v>30</v>
@@ -3801,7 +3675,7 @@
         <v>31</v>
       </c>
       <c r="S40" t="s">
-        <v>151</v>
+        <v>32</v>
       </c>
     </row>
     <row r="41" spans="1:19" x14ac:dyDescent="0.2">
@@ -3839,6 +3713,9 @@
         <f t="shared" si="3"/>
         <v>GRCh38_HPRC-HG02717_dipz2k</v>
       </c>
+      <c r="K41" t="s">
+        <v>24</v>
+      </c>
       <c r="L41" t="s">
         <v>25</v>
       </c>
@@ -3853,7 +3730,7 @@
         <v>HPRC-HG02717</v>
       </c>
       <c r="P41" t="s">
-        <v>152</v>
+        <v>29</v>
       </c>
       <c r="Q41" t="s">
         <v>30</v>
@@ -3862,7 +3739,7 @@
         <v>31</v>
       </c>
       <c r="S41" t="s">
-        <v>153</v>
+        <v>32</v>
       </c>
     </row>
     <row r="42" spans="1:19" x14ac:dyDescent="0.2">
@@ -3900,6 +3777,9 @@
         <f t="shared" si="3"/>
         <v>GRCh38_HPRC-HG02886_dipz2k</v>
       </c>
+      <c r="K42" t="s">
+        <v>24</v>
+      </c>
       <c r="L42" t="s">
         <v>25</v>
       </c>
@@ -3914,7 +3794,7 @@
         <v>HPRC-HG02886</v>
       </c>
       <c r="P42" t="s">
-        <v>154</v>
+        <v>29</v>
       </c>
       <c r="Q42" t="s">
         <v>30</v>
@@ -3923,7 +3803,7 @@
         <v>31</v>
       </c>
       <c r="S42" t="s">
-        <v>155</v>
+        <v>32</v>
       </c>
     </row>
     <row r="43" spans="1:19" x14ac:dyDescent="0.2">
@@ -3961,6 +3841,9 @@
         <f t="shared" si="3"/>
         <v>GRCh38_HPRC-HG03453_dipz2k</v>
       </c>
+      <c r="K43" t="s">
+        <v>24</v>
+      </c>
       <c r="L43" t="s">
         <v>25</v>
       </c>
@@ -3975,7 +3858,7 @@
         <v>HPRC-HG03453</v>
       </c>
       <c r="P43" t="s">
-        <v>156</v>
+        <v>29</v>
       </c>
       <c r="Q43" t="s">
         <v>30</v>
@@ -3984,7 +3867,7 @@
         <v>31</v>
       </c>
       <c r="S43" t="s">
-        <v>157</v>
+        <v>32</v>
       </c>
     </row>
     <row r="44" spans="1:19" x14ac:dyDescent="0.2">
@@ -4022,6 +3905,9 @@
         <f t="shared" si="3"/>
         <v>GRCh38_HPRC-HG03516_dipz2k</v>
       </c>
+      <c r="K44" t="s">
+        <v>24</v>
+      </c>
       <c r="L44" t="s">
         <v>25</v>
       </c>
@@ -4036,7 +3922,7 @@
         <v>HPRC-HG03516</v>
       </c>
       <c r="P44" t="s">
-        <v>158</v>
+        <v>29</v>
       </c>
       <c r="Q44" t="s">
         <v>30</v>
@@ -4045,7 +3931,7 @@
         <v>31</v>
       </c>
       <c r="S44" t="s">
-        <v>159</v>
+        <v>32</v>
       </c>
     </row>
     <row r="45" spans="1:19" x14ac:dyDescent="0.2">
@@ -4083,6 +3969,9 @@
         <f t="shared" si="3"/>
         <v>GRCh38_HPRC-HG03540_dipz2k</v>
       </c>
+      <c r="K45" t="s">
+        <v>24</v>
+      </c>
       <c r="L45" t="s">
         <v>25</v>
       </c>
@@ -4097,7 +3986,7 @@
         <v>HPRC-HG03540</v>
       </c>
       <c r="P45" t="s">
-        <v>160</v>
+        <v>29</v>
       </c>
       <c r="Q45" t="s">
         <v>30</v>
@@ -4106,7 +3995,7 @@
         <v>31</v>
       </c>
       <c r="S45" t="s">
-        <v>161</v>
+        <v>32</v>
       </c>
     </row>
     <row r="46" spans="1:19" x14ac:dyDescent="0.2">
@@ -4144,6 +4033,9 @@
         <f>CONCATENATE("GRCh38_HPRC-",A46,"_dipz2k")</f>
         <v>GRCh38_HPRC-HG03579_dipz2k</v>
       </c>
+      <c r="K46" t="s">
+        <v>24</v>
+      </c>
       <c r="L46" t="s">
         <v>25</v>
       </c>
@@ -4158,7 +4050,7 @@
         <v>HPRC-HG03579</v>
       </c>
       <c r="P46" t="s">
-        <v>162</v>
+        <v>29</v>
       </c>
       <c r="Q46" t="s">
         <v>30</v>
@@ -4167,7 +4059,2439 @@
         <v>31</v>
       </c>
       <c r="S46" t="s">
-        <v>163</v>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="47" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A47" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B47" t="str">
+        <f>CONCATENATE("GRCh38_T~HPRC-",A47,"-dipz2k_Q~ILMNDV-",A47)</f>
+        <v>GRCh38_T~HPRC-HG00438-dipz2k_Q~ILMNDV-HG00438</v>
+      </c>
+      <c r="C47" t="str">
+        <f>CONCATENATE("GRCh38_HPRC-", A47,"-dipz2k_smvar-excluded")</f>
+        <v>GRCh38_HPRC-HG00438-dipz2k_smvar-excluded</v>
+      </c>
+      <c r="D47" t="s">
+        <v>20</v>
+      </c>
+      <c r="E47" t="s">
+        <v>21</v>
+      </c>
+      <c r="F47" t="str">
+        <f>CONCATENATE("ILMN-DV-",A47)</f>
+        <v>ILMN-DV-HG00438</v>
+      </c>
+      <c r="G47" t="b">
+        <v>0</v>
+      </c>
+      <c r="H47" t="b">
+        <v>1</v>
+      </c>
+      <c r="I47" t="s">
+        <v>33</v>
+      </c>
+      <c r="J47" t="str">
+        <f>CONCATENATE("GRCh38_HPRC-",A47,"_dipz2k")</f>
+        <v>GRCh38_HPRC-HG00438_dipz2k</v>
+      </c>
+      <c r="K47" t="s">
+        <v>24</v>
+      </c>
+      <c r="L47" t="s">
+        <v>25</v>
+      </c>
+      <c r="M47" t="s">
+        <v>26</v>
+      </c>
+      <c r="N47" t="s">
+        <v>27</v>
+      </c>
+      <c r="O47" t="str">
+        <f>CONCATENATE("HPRC-",A47)</f>
+        <v>HPRC-HG00438</v>
+      </c>
+      <c r="P47" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q47" t="s">
+        <v>30</v>
+      </c>
+      <c r="R47" t="s">
+        <v>31</v>
+      </c>
+      <c r="S47" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="48" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>50</v>
+      </c>
+      <c r="B48" t="str">
+        <f t="shared" ref="B48:B84" si="5">CONCATENATE("GRCh38_T~HPRC-",A48,"-dipz2k_Q~ILMNDV-",A48)</f>
+        <v>GRCh38_T~HPRC-HG00621-dipz2k_Q~ILMNDV-HG00621</v>
+      </c>
+      <c r="C48" t="str">
+        <f t="shared" ref="C48:C84" si="6">CONCATENATE("GRCh38_HPRC-", A48,"-dipz2k_smvar-excluded")</f>
+        <v>GRCh38_HPRC-HG00621-dipz2k_smvar-excluded</v>
+      </c>
+      <c r="D48" t="s">
+        <v>20</v>
+      </c>
+      <c r="E48" t="s">
+        <v>21</v>
+      </c>
+      <c r="F48" t="str">
+        <f t="shared" ref="F48:F84" si="7">CONCATENATE("ILMN-DV-",A48)</f>
+        <v>ILMN-DV-HG00621</v>
+      </c>
+      <c r="G48" t="b">
+        <v>0</v>
+      </c>
+      <c r="H48" t="b">
+        <v>1</v>
+      </c>
+      <c r="I48" t="s">
+        <v>33</v>
+      </c>
+      <c r="J48" t="str">
+        <f t="shared" ref="J48:J84" si="8">CONCATENATE("GRCh38_HPRC-",A48,"_dipz2k")</f>
+        <v>GRCh38_HPRC-HG00621_dipz2k</v>
+      </c>
+      <c r="K48" t="s">
+        <v>24</v>
+      </c>
+      <c r="L48" t="s">
+        <v>25</v>
+      </c>
+      <c r="M48" t="s">
+        <v>26</v>
+      </c>
+      <c r="N48" t="s">
+        <v>27</v>
+      </c>
+      <c r="O48" t="str">
+        <f t="shared" ref="O48:O84" si="9">CONCATENATE("HPRC-",A48)</f>
+        <v>HPRC-HG00621</v>
+      </c>
+      <c r="P48" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q48" t="s">
+        <v>30</v>
+      </c>
+      <c r="R48" t="s">
+        <v>31</v>
+      </c>
+      <c r="S48" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="49" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>51</v>
+      </c>
+      <c r="B49" t="str">
+        <f t="shared" si="5"/>
+        <v>GRCh38_T~HPRC-HG00673-dipz2k_Q~ILMNDV-HG00673</v>
+      </c>
+      <c r="C49" t="str">
+        <f t="shared" si="6"/>
+        <v>GRCh38_HPRC-HG00673-dipz2k_smvar-excluded</v>
+      </c>
+      <c r="D49" t="s">
+        <v>20</v>
+      </c>
+      <c r="E49" t="s">
+        <v>21</v>
+      </c>
+      <c r="F49" t="str">
+        <f t="shared" si="7"/>
+        <v>ILMN-DV-HG00673</v>
+      </c>
+      <c r="G49" t="b">
+        <v>0</v>
+      </c>
+      <c r="H49" t="b">
+        <v>1</v>
+      </c>
+      <c r="I49" t="s">
+        <v>33</v>
+      </c>
+      <c r="J49" t="str">
+        <f t="shared" si="8"/>
+        <v>GRCh38_HPRC-HG00673_dipz2k</v>
+      </c>
+      <c r="K49" t="s">
+        <v>24</v>
+      </c>
+      <c r="L49" t="s">
+        <v>25</v>
+      </c>
+      <c r="M49" t="s">
+        <v>26</v>
+      </c>
+      <c r="N49" t="s">
+        <v>27</v>
+      </c>
+      <c r="O49" t="str">
+        <f t="shared" si="9"/>
+        <v>HPRC-HG00673</v>
+      </c>
+      <c r="P49" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q49" t="s">
+        <v>30</v>
+      </c>
+      <c r="R49" t="s">
+        <v>31</v>
+      </c>
+      <c r="S49" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="50" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>34</v>
+      </c>
+      <c r="B50" t="str">
+        <f t="shared" si="5"/>
+        <v>GRCh38_T~HPRC-HG00733-dipz2k_Q~ILMNDV-HG00733</v>
+      </c>
+      <c r="C50" t="str">
+        <f t="shared" si="6"/>
+        <v>GRCh38_HPRC-HG00733-dipz2k_smvar-excluded</v>
+      </c>
+      <c r="D50" t="s">
+        <v>20</v>
+      </c>
+      <c r="E50" t="s">
+        <v>21</v>
+      </c>
+      <c r="F50" t="str">
+        <f t="shared" si="7"/>
+        <v>ILMN-DV-HG00733</v>
+      </c>
+      <c r="G50" t="b">
+        <v>0</v>
+      </c>
+      <c r="H50" t="b">
+        <v>1</v>
+      </c>
+      <c r="I50" t="s">
+        <v>33</v>
+      </c>
+      <c r="J50" t="str">
+        <f t="shared" si="8"/>
+        <v>GRCh38_HPRC-HG00733_dipz2k</v>
+      </c>
+      <c r="K50" t="s">
+        <v>24</v>
+      </c>
+      <c r="L50" t="s">
+        <v>25</v>
+      </c>
+      <c r="M50" t="s">
+        <v>26</v>
+      </c>
+      <c r="N50" t="s">
+        <v>27</v>
+      </c>
+      <c r="O50" t="str">
+        <f t="shared" si="9"/>
+        <v>HPRC-HG00733</v>
+      </c>
+      <c r="P50" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q50" t="s">
+        <v>30</v>
+      </c>
+      <c r="R50" t="s">
+        <v>31</v>
+      </c>
+      <c r="S50" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="51" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>52</v>
+      </c>
+      <c r="B51" t="str">
+        <f t="shared" si="5"/>
+        <v>GRCh38_T~HPRC-HG00735-dipz2k_Q~ILMNDV-HG00735</v>
+      </c>
+      <c r="C51" t="str">
+        <f t="shared" si="6"/>
+        <v>GRCh38_HPRC-HG00735-dipz2k_smvar-excluded</v>
+      </c>
+      <c r="D51" t="s">
+        <v>20</v>
+      </c>
+      <c r="E51" t="s">
+        <v>21</v>
+      </c>
+      <c r="F51" t="str">
+        <f t="shared" si="7"/>
+        <v>ILMN-DV-HG00735</v>
+      </c>
+      <c r="G51" t="b">
+        <v>0</v>
+      </c>
+      <c r="H51" t="b">
+        <v>1</v>
+      </c>
+      <c r="I51" t="s">
+        <v>33</v>
+      </c>
+      <c r="J51" t="str">
+        <f t="shared" si="8"/>
+        <v>GRCh38_HPRC-HG00735_dipz2k</v>
+      </c>
+      <c r="K51" t="s">
+        <v>24</v>
+      </c>
+      <c r="L51" t="s">
+        <v>25</v>
+      </c>
+      <c r="M51" t="s">
+        <v>26</v>
+      </c>
+      <c r="N51" t="s">
+        <v>27</v>
+      </c>
+      <c r="O51" t="str">
+        <f t="shared" si="9"/>
+        <v>HPRC-HG00735</v>
+      </c>
+      <c r="P51" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q51" t="s">
+        <v>30</v>
+      </c>
+      <c r="R51" t="s">
+        <v>31</v>
+      </c>
+      <c r="S51" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="52" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>53</v>
+      </c>
+      <c r="B52" t="str">
+        <f t="shared" si="5"/>
+        <v>GRCh38_T~HPRC-HG00741-dipz2k_Q~ILMNDV-HG00741</v>
+      </c>
+      <c r="C52" t="str">
+        <f t="shared" si="6"/>
+        <v>GRCh38_HPRC-HG00741-dipz2k_smvar-excluded</v>
+      </c>
+      <c r="D52" t="s">
+        <v>20</v>
+      </c>
+      <c r="E52" t="s">
+        <v>21</v>
+      </c>
+      <c r="F52" t="str">
+        <f t="shared" si="7"/>
+        <v>ILMN-DV-HG00741</v>
+      </c>
+      <c r="G52" t="b">
+        <v>0</v>
+      </c>
+      <c r="H52" t="b">
+        <v>1</v>
+      </c>
+      <c r="I52" t="s">
+        <v>33</v>
+      </c>
+      <c r="J52" t="str">
+        <f t="shared" si="8"/>
+        <v>GRCh38_HPRC-HG00741_dipz2k</v>
+      </c>
+      <c r="K52" t="s">
+        <v>24</v>
+      </c>
+      <c r="L52" t="s">
+        <v>25</v>
+      </c>
+      <c r="M52" t="s">
+        <v>26</v>
+      </c>
+      <c r="N52" t="s">
+        <v>27</v>
+      </c>
+      <c r="O52" t="str">
+        <f t="shared" si="9"/>
+        <v>HPRC-HG00741</v>
+      </c>
+      <c r="P52" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q52" t="s">
+        <v>30</v>
+      </c>
+      <c r="R52" t="s">
+        <v>31</v>
+      </c>
+      <c r="S52" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="53" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>54</v>
+      </c>
+      <c r="B53" t="str">
+        <f t="shared" si="5"/>
+        <v>GRCh38_T~HPRC-HG01071-dipz2k_Q~ILMNDV-HG01071</v>
+      </c>
+      <c r="C53" t="str">
+        <f t="shared" si="6"/>
+        <v>GRCh38_HPRC-HG01071-dipz2k_smvar-excluded</v>
+      </c>
+      <c r="D53" t="s">
+        <v>20</v>
+      </c>
+      <c r="E53" t="s">
+        <v>21</v>
+      </c>
+      <c r="F53" t="str">
+        <f t="shared" si="7"/>
+        <v>ILMN-DV-HG01071</v>
+      </c>
+      <c r="G53" t="b">
+        <v>0</v>
+      </c>
+      <c r="H53" t="b">
+        <v>1</v>
+      </c>
+      <c r="I53" t="s">
+        <v>33</v>
+      </c>
+      <c r="J53" t="str">
+        <f t="shared" si="8"/>
+        <v>GRCh38_HPRC-HG01071_dipz2k</v>
+      </c>
+      <c r="K53" t="s">
+        <v>24</v>
+      </c>
+      <c r="L53" t="s">
+        <v>25</v>
+      </c>
+      <c r="M53" t="s">
+        <v>26</v>
+      </c>
+      <c r="N53" t="s">
+        <v>27</v>
+      </c>
+      <c r="O53" t="str">
+        <f t="shared" si="9"/>
+        <v>HPRC-HG01071</v>
+      </c>
+      <c r="P53" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q53" t="s">
+        <v>30</v>
+      </c>
+      <c r="R53" t="s">
+        <v>31</v>
+      </c>
+      <c r="S53" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="54" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>55</v>
+      </c>
+      <c r="B54" t="str">
+        <f t="shared" si="5"/>
+        <v>GRCh38_T~HPRC-HG01106-dipz2k_Q~ILMNDV-HG01106</v>
+      </c>
+      <c r="C54" t="str">
+        <f t="shared" si="6"/>
+        <v>GRCh38_HPRC-HG01106-dipz2k_smvar-excluded</v>
+      </c>
+      <c r="D54" t="s">
+        <v>20</v>
+      </c>
+      <c r="E54" t="s">
+        <v>21</v>
+      </c>
+      <c r="F54" t="str">
+        <f t="shared" si="7"/>
+        <v>ILMN-DV-HG01106</v>
+      </c>
+      <c r="G54" t="b">
+        <v>0</v>
+      </c>
+      <c r="H54" t="b">
+        <v>1</v>
+      </c>
+      <c r="I54" t="s">
+        <v>33</v>
+      </c>
+      <c r="J54" t="str">
+        <f t="shared" si="8"/>
+        <v>GRCh38_HPRC-HG01106_dipz2k</v>
+      </c>
+      <c r="K54" t="s">
+        <v>24</v>
+      </c>
+      <c r="L54" t="s">
+        <v>25</v>
+      </c>
+      <c r="M54" t="s">
+        <v>26</v>
+      </c>
+      <c r="N54" t="s">
+        <v>27</v>
+      </c>
+      <c r="O54" t="str">
+        <f t="shared" si="9"/>
+        <v>HPRC-HG01106</v>
+      </c>
+      <c r="P54" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q54" t="s">
+        <v>30</v>
+      </c>
+      <c r="R54" t="s">
+        <v>31</v>
+      </c>
+      <c r="S54" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="55" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>35</v>
+      </c>
+      <c r="B55" t="str">
+        <f t="shared" si="5"/>
+        <v>GRCh38_T~HPRC-HG01109-dipz2k_Q~ILMNDV-HG01109</v>
+      </c>
+      <c r="C55" t="str">
+        <f t="shared" si="6"/>
+        <v>GRCh38_HPRC-HG01109-dipz2k_smvar-excluded</v>
+      </c>
+      <c r="D55" t="s">
+        <v>20</v>
+      </c>
+      <c r="E55" t="s">
+        <v>21</v>
+      </c>
+      <c r="F55" t="str">
+        <f t="shared" si="7"/>
+        <v>ILMN-DV-HG01109</v>
+      </c>
+      <c r="G55" t="b">
+        <v>0</v>
+      </c>
+      <c r="H55" t="b">
+        <v>1</v>
+      </c>
+      <c r="I55" t="s">
+        <v>33</v>
+      </c>
+      <c r="J55" t="str">
+        <f t="shared" si="8"/>
+        <v>GRCh38_HPRC-HG01109_dipz2k</v>
+      </c>
+      <c r="K55" t="s">
+        <v>24</v>
+      </c>
+      <c r="L55" t="s">
+        <v>25</v>
+      </c>
+      <c r="M55" t="s">
+        <v>26</v>
+      </c>
+      <c r="N55" t="s">
+        <v>27</v>
+      </c>
+      <c r="O55" t="str">
+        <f t="shared" si="9"/>
+        <v>HPRC-HG01109</v>
+      </c>
+      <c r="P55" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q55" t="s">
+        <v>30</v>
+      </c>
+      <c r="R55" t="s">
+        <v>31</v>
+      </c>
+      <c r="S55" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="56" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>57</v>
+      </c>
+      <c r="B56" t="str">
+        <f t="shared" si="5"/>
+        <v>GRCh38_T~HPRC-HG01175-dipz2k_Q~ILMNDV-HG01175</v>
+      </c>
+      <c r="C56" t="str">
+        <f t="shared" si="6"/>
+        <v>GRCh38_HPRC-HG01175-dipz2k_smvar-excluded</v>
+      </c>
+      <c r="D56" t="s">
+        <v>20</v>
+      </c>
+      <c r="E56" t="s">
+        <v>21</v>
+      </c>
+      <c r="F56" t="str">
+        <f t="shared" si="7"/>
+        <v>ILMN-DV-HG01175</v>
+      </c>
+      <c r="G56" t="b">
+        <v>0</v>
+      </c>
+      <c r="H56" t="b">
+        <v>1</v>
+      </c>
+      <c r="I56" t="s">
+        <v>33</v>
+      </c>
+      <c r="J56" t="str">
+        <f t="shared" si="8"/>
+        <v>GRCh38_HPRC-HG01175_dipz2k</v>
+      </c>
+      <c r="K56" t="s">
+        <v>24</v>
+      </c>
+      <c r="L56" t="s">
+        <v>25</v>
+      </c>
+      <c r="M56" t="s">
+        <v>26</v>
+      </c>
+      <c r="N56" t="s">
+        <v>27</v>
+      </c>
+      <c r="O56" t="str">
+        <f t="shared" si="9"/>
+        <v>HPRC-HG01175</v>
+      </c>
+      <c r="P56" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q56" t="s">
+        <v>30</v>
+      </c>
+      <c r="R56" t="s">
+        <v>31</v>
+      </c>
+      <c r="S56" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="57" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>36</v>
+      </c>
+      <c r="B57" t="str">
+        <f t="shared" si="5"/>
+        <v>GRCh38_T~HPRC-HG01243-dipz2k_Q~ILMNDV-HG01243</v>
+      </c>
+      <c r="C57" t="str">
+        <f t="shared" si="6"/>
+        <v>GRCh38_HPRC-HG01243-dipz2k_smvar-excluded</v>
+      </c>
+      <c r="D57" t="s">
+        <v>20</v>
+      </c>
+      <c r="E57" t="s">
+        <v>21</v>
+      </c>
+      <c r="F57" t="str">
+        <f t="shared" si="7"/>
+        <v>ILMN-DV-HG01243</v>
+      </c>
+      <c r="G57" t="b">
+        <v>0</v>
+      </c>
+      <c r="H57" t="b">
+        <v>1</v>
+      </c>
+      <c r="I57" t="s">
+        <v>33</v>
+      </c>
+      <c r="J57" t="str">
+        <f t="shared" si="8"/>
+        <v>GRCh38_HPRC-HG01243_dipz2k</v>
+      </c>
+      <c r="K57" t="s">
+        <v>24</v>
+      </c>
+      <c r="L57" t="s">
+        <v>25</v>
+      </c>
+      <c r="M57" t="s">
+        <v>26</v>
+      </c>
+      <c r="N57" t="s">
+        <v>27</v>
+      </c>
+      <c r="O57" t="str">
+        <f t="shared" si="9"/>
+        <v>HPRC-HG01243</v>
+      </c>
+      <c r="P57" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q57" t="s">
+        <v>30</v>
+      </c>
+      <c r="R57" t="s">
+        <v>31</v>
+      </c>
+      <c r="S57" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="58" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>58</v>
+      </c>
+      <c r="B58" t="str">
+        <f t="shared" si="5"/>
+        <v>GRCh38_T~HPRC-HG01258-dipz2k_Q~ILMNDV-HG01258</v>
+      </c>
+      <c r="C58" t="str">
+        <f t="shared" si="6"/>
+        <v>GRCh38_HPRC-HG01258-dipz2k_smvar-excluded</v>
+      </c>
+      <c r="D58" t="s">
+        <v>20</v>
+      </c>
+      <c r="E58" t="s">
+        <v>21</v>
+      </c>
+      <c r="F58" t="str">
+        <f t="shared" si="7"/>
+        <v>ILMN-DV-HG01258</v>
+      </c>
+      <c r="G58" t="b">
+        <v>0</v>
+      </c>
+      <c r="H58" t="b">
+        <v>1</v>
+      </c>
+      <c r="I58" t="s">
+        <v>33</v>
+      </c>
+      <c r="J58" t="str">
+        <f t="shared" si="8"/>
+        <v>GRCh38_HPRC-HG01258_dipz2k</v>
+      </c>
+      <c r="K58" t="s">
+        <v>24</v>
+      </c>
+      <c r="L58" t="s">
+        <v>25</v>
+      </c>
+      <c r="M58" t="s">
+        <v>26</v>
+      </c>
+      <c r="N58" t="s">
+        <v>27</v>
+      </c>
+      <c r="O58" t="str">
+        <f t="shared" si="9"/>
+        <v>HPRC-HG01258</v>
+      </c>
+      <c r="P58" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q58" t="s">
+        <v>30</v>
+      </c>
+      <c r="R58" t="s">
+        <v>31</v>
+      </c>
+      <c r="S58" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="59" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>59</v>
+      </c>
+      <c r="B59" t="str">
+        <f t="shared" si="5"/>
+        <v>GRCh38_T~HPRC-HG01358-dipz2k_Q~ILMNDV-HG01358</v>
+      </c>
+      <c r="C59" t="str">
+        <f t="shared" si="6"/>
+        <v>GRCh38_HPRC-HG01358-dipz2k_smvar-excluded</v>
+      </c>
+      <c r="D59" t="s">
+        <v>20</v>
+      </c>
+      <c r="E59" t="s">
+        <v>21</v>
+      </c>
+      <c r="F59" t="str">
+        <f t="shared" si="7"/>
+        <v>ILMN-DV-HG01358</v>
+      </c>
+      <c r="G59" t="b">
+        <v>0</v>
+      </c>
+      <c r="H59" t="b">
+        <v>1</v>
+      </c>
+      <c r="I59" t="s">
+        <v>33</v>
+      </c>
+      <c r="J59" t="str">
+        <f t="shared" si="8"/>
+        <v>GRCh38_HPRC-HG01358_dipz2k</v>
+      </c>
+      <c r="K59" t="s">
+        <v>24</v>
+      </c>
+      <c r="L59" t="s">
+        <v>25</v>
+      </c>
+      <c r="M59" t="s">
+        <v>26</v>
+      </c>
+      <c r="N59" t="s">
+        <v>27</v>
+      </c>
+      <c r="O59" t="str">
+        <f t="shared" si="9"/>
+        <v>HPRC-HG01358</v>
+      </c>
+      <c r="P59" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q59" t="s">
+        <v>30</v>
+      </c>
+      <c r="R59" t="s">
+        <v>31</v>
+      </c>
+      <c r="S59" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="60" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>60</v>
+      </c>
+      <c r="B60" t="str">
+        <f t="shared" si="5"/>
+        <v>GRCh38_T~HPRC-HG01361-dipz2k_Q~ILMNDV-HG01361</v>
+      </c>
+      <c r="C60" t="str">
+        <f t="shared" si="6"/>
+        <v>GRCh38_HPRC-HG01361-dipz2k_smvar-excluded</v>
+      </c>
+      <c r="D60" t="s">
+        <v>20</v>
+      </c>
+      <c r="E60" t="s">
+        <v>21</v>
+      </c>
+      <c r="F60" t="str">
+        <f t="shared" si="7"/>
+        <v>ILMN-DV-HG01361</v>
+      </c>
+      <c r="G60" t="b">
+        <v>0</v>
+      </c>
+      <c r="H60" t="b">
+        <v>1</v>
+      </c>
+      <c r="I60" t="s">
+        <v>33</v>
+      </c>
+      <c r="J60" t="str">
+        <f t="shared" si="8"/>
+        <v>GRCh38_HPRC-HG01361_dipz2k</v>
+      </c>
+      <c r="K60" t="s">
+        <v>24</v>
+      </c>
+      <c r="L60" t="s">
+        <v>25</v>
+      </c>
+      <c r="M60" t="s">
+        <v>26</v>
+      </c>
+      <c r="N60" t="s">
+        <v>27</v>
+      </c>
+      <c r="O60" t="str">
+        <f t="shared" si="9"/>
+        <v>HPRC-HG01361</v>
+      </c>
+      <c r="P60" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q60" t="s">
+        <v>30</v>
+      </c>
+      <c r="R60" t="s">
+        <v>31</v>
+      </c>
+      <c r="S60" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="61" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>61</v>
+      </c>
+      <c r="B61" t="str">
+        <f t="shared" si="5"/>
+        <v>GRCh38_T~HPRC-HG01891-dipz2k_Q~ILMNDV-HG01891</v>
+      </c>
+      <c r="C61" t="str">
+        <f t="shared" si="6"/>
+        <v>GRCh38_HPRC-HG01891-dipz2k_smvar-excluded</v>
+      </c>
+      <c r="D61" t="s">
+        <v>20</v>
+      </c>
+      <c r="E61" t="s">
+        <v>21</v>
+      </c>
+      <c r="F61" t="str">
+        <f t="shared" si="7"/>
+        <v>ILMN-DV-HG01891</v>
+      </c>
+      <c r="G61" t="b">
+        <v>0</v>
+      </c>
+      <c r="H61" t="b">
+        <v>1</v>
+      </c>
+      <c r="I61" t="s">
+        <v>33</v>
+      </c>
+      <c r="J61" t="str">
+        <f t="shared" si="8"/>
+        <v>GRCh38_HPRC-HG01891_dipz2k</v>
+      </c>
+      <c r="K61" t="s">
+        <v>24</v>
+      </c>
+      <c r="L61" t="s">
+        <v>25</v>
+      </c>
+      <c r="M61" t="s">
+        <v>26</v>
+      </c>
+      <c r="N61" t="s">
+        <v>27</v>
+      </c>
+      <c r="O61" t="str">
+        <f t="shared" si="9"/>
+        <v>HPRC-HG01891</v>
+      </c>
+      <c r="P61" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q61" t="s">
+        <v>30</v>
+      </c>
+      <c r="R61" t="s">
+        <v>31</v>
+      </c>
+      <c r="S61" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="62" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>62</v>
+      </c>
+      <c r="B62" t="str">
+        <f t="shared" si="5"/>
+        <v>GRCh38_T~HPRC-HG01928-dipz2k_Q~ILMNDV-HG01928</v>
+      </c>
+      <c r="C62" t="str">
+        <f t="shared" si="6"/>
+        <v>GRCh38_HPRC-HG01928-dipz2k_smvar-excluded</v>
+      </c>
+      <c r="D62" t="s">
+        <v>20</v>
+      </c>
+      <c r="E62" t="s">
+        <v>21</v>
+      </c>
+      <c r="F62" t="str">
+        <f t="shared" si="7"/>
+        <v>ILMN-DV-HG01928</v>
+      </c>
+      <c r="G62" t="b">
+        <v>0</v>
+      </c>
+      <c r="H62" t="b">
+        <v>1</v>
+      </c>
+      <c r="I62" t="s">
+        <v>33</v>
+      </c>
+      <c r="J62" t="str">
+        <f t="shared" si="8"/>
+        <v>GRCh38_HPRC-HG01928_dipz2k</v>
+      </c>
+      <c r="K62" t="s">
+        <v>24</v>
+      </c>
+      <c r="L62" t="s">
+        <v>25</v>
+      </c>
+      <c r="M62" t="s">
+        <v>26</v>
+      </c>
+      <c r="N62" t="s">
+        <v>27</v>
+      </c>
+      <c r="O62" t="str">
+        <f t="shared" si="9"/>
+        <v>HPRC-HG01928</v>
+      </c>
+      <c r="P62" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q62" t="s">
+        <v>30</v>
+      </c>
+      <c r="R62" t="s">
+        <v>31</v>
+      </c>
+      <c r="S62" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="63" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>63</v>
+      </c>
+      <c r="B63" t="str">
+        <f t="shared" si="5"/>
+        <v>GRCh38_T~HPRC-HG01952-dipz2k_Q~ILMNDV-HG01952</v>
+      </c>
+      <c r="C63" t="str">
+        <f t="shared" si="6"/>
+        <v>GRCh38_HPRC-HG01952-dipz2k_smvar-excluded</v>
+      </c>
+      <c r="D63" t="s">
+        <v>20</v>
+      </c>
+      <c r="E63" t="s">
+        <v>21</v>
+      </c>
+      <c r="F63" t="str">
+        <f t="shared" si="7"/>
+        <v>ILMN-DV-HG01952</v>
+      </c>
+      <c r="G63" t="b">
+        <v>0</v>
+      </c>
+      <c r="H63" t="b">
+        <v>1</v>
+      </c>
+      <c r="I63" t="s">
+        <v>33</v>
+      </c>
+      <c r="J63" t="str">
+        <f t="shared" si="8"/>
+        <v>GRCh38_HPRC-HG01952_dipz2k</v>
+      </c>
+      <c r="K63" t="s">
+        <v>24</v>
+      </c>
+      <c r="L63" t="s">
+        <v>25</v>
+      </c>
+      <c r="M63" t="s">
+        <v>26</v>
+      </c>
+      <c r="N63" t="s">
+        <v>27</v>
+      </c>
+      <c r="O63" t="str">
+        <f t="shared" si="9"/>
+        <v>HPRC-HG01952</v>
+      </c>
+      <c r="P63" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q63" t="s">
+        <v>30</v>
+      </c>
+      <c r="R63" t="s">
+        <v>31</v>
+      </c>
+      <c r="S63" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="64" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>64</v>
+      </c>
+      <c r="B64" t="str">
+        <f t="shared" si="5"/>
+        <v>GRCh38_T~HPRC-HG01978-dipz2k_Q~ILMNDV-HG01978</v>
+      </c>
+      <c r="C64" t="str">
+        <f t="shared" si="6"/>
+        <v>GRCh38_HPRC-HG01978-dipz2k_smvar-excluded</v>
+      </c>
+      <c r="D64" t="s">
+        <v>20</v>
+      </c>
+      <c r="E64" t="s">
+        <v>21</v>
+      </c>
+      <c r="F64" t="str">
+        <f t="shared" si="7"/>
+        <v>ILMN-DV-HG01978</v>
+      </c>
+      <c r="G64" t="b">
+        <v>0</v>
+      </c>
+      <c r="H64" t="b">
+        <v>1</v>
+      </c>
+      <c r="I64" t="s">
+        <v>33</v>
+      </c>
+      <c r="J64" t="str">
+        <f t="shared" si="8"/>
+        <v>GRCh38_HPRC-HG01978_dipz2k</v>
+      </c>
+      <c r="K64" t="s">
+        <v>24</v>
+      </c>
+      <c r="L64" t="s">
+        <v>25</v>
+      </c>
+      <c r="M64" t="s">
+        <v>26</v>
+      </c>
+      <c r="N64" t="s">
+        <v>27</v>
+      </c>
+      <c r="O64" t="str">
+        <f t="shared" si="9"/>
+        <v>HPRC-HG01978</v>
+      </c>
+      <c r="P64" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q64" t="s">
+        <v>30</v>
+      </c>
+      <c r="R64" t="s">
+        <v>31</v>
+      </c>
+      <c r="S64" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="65" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>37</v>
+      </c>
+      <c r="B65" t="str">
+        <f t="shared" si="5"/>
+        <v>GRCh38_T~HPRC-HG02055-dipz2k_Q~ILMNDV-HG02055</v>
+      </c>
+      <c r="C65" t="str">
+        <f t="shared" si="6"/>
+        <v>GRCh38_HPRC-HG02055-dipz2k_smvar-excluded</v>
+      </c>
+      <c r="D65" t="s">
+        <v>20</v>
+      </c>
+      <c r="E65" t="s">
+        <v>21</v>
+      </c>
+      <c r="F65" t="str">
+        <f t="shared" si="7"/>
+        <v>ILMN-DV-HG02055</v>
+      </c>
+      <c r="G65" t="b">
+        <v>0</v>
+      </c>
+      <c r="H65" t="b">
+        <v>1</v>
+      </c>
+      <c r="I65" t="s">
+        <v>33</v>
+      </c>
+      <c r="J65" t="str">
+        <f t="shared" si="8"/>
+        <v>GRCh38_HPRC-HG02055_dipz2k</v>
+      </c>
+      <c r="K65" t="s">
+        <v>24</v>
+      </c>
+      <c r="L65" t="s">
+        <v>25</v>
+      </c>
+      <c r="M65" t="s">
+        <v>26</v>
+      </c>
+      <c r="N65" t="s">
+        <v>27</v>
+      </c>
+      <c r="O65" t="str">
+        <f t="shared" si="9"/>
+        <v>HPRC-HG02055</v>
+      </c>
+      <c r="P65" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q65" t="s">
+        <v>30</v>
+      </c>
+      <c r="R65" t="s">
+        <v>31</v>
+      </c>
+      <c r="S65" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="66" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>38</v>
+      </c>
+      <c r="B66" t="str">
+        <f t="shared" si="5"/>
+        <v>GRCh38_T~HPRC-HG02080-dipz2k_Q~ILMNDV-HG02080</v>
+      </c>
+      <c r="C66" t="str">
+        <f t="shared" si="6"/>
+        <v>GRCh38_HPRC-HG02080-dipz2k_smvar-excluded</v>
+      </c>
+      <c r="D66" t="s">
+        <v>20</v>
+      </c>
+      <c r="E66" t="s">
+        <v>21</v>
+      </c>
+      <c r="F66" t="str">
+        <f t="shared" si="7"/>
+        <v>ILMN-DV-HG02080</v>
+      </c>
+      <c r="G66" t="b">
+        <v>0</v>
+      </c>
+      <c r="H66" t="b">
+        <v>1</v>
+      </c>
+      <c r="I66" t="s">
+        <v>33</v>
+      </c>
+      <c r="J66" t="str">
+        <f t="shared" si="8"/>
+        <v>GRCh38_HPRC-HG02080_dipz2k</v>
+      </c>
+      <c r="K66" t="s">
+        <v>24</v>
+      </c>
+      <c r="L66" t="s">
+        <v>25</v>
+      </c>
+      <c r="M66" t="s">
+        <v>26</v>
+      </c>
+      <c r="N66" t="s">
+        <v>27</v>
+      </c>
+      <c r="O66" t="str">
+        <f t="shared" si="9"/>
+        <v>HPRC-HG02080</v>
+      </c>
+      <c r="P66" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q66" t="s">
+        <v>30</v>
+      </c>
+      <c r="R66" t="s">
+        <v>31</v>
+      </c>
+      <c r="S66" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="67" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>40</v>
+      </c>
+      <c r="B67" t="str">
+        <f t="shared" si="5"/>
+        <v>GRCh38_T~HPRC-HG02145-dipz2k_Q~ILMNDV-HG02145</v>
+      </c>
+      <c r="C67" t="str">
+        <f t="shared" si="6"/>
+        <v>GRCh38_HPRC-HG02145-dipz2k_smvar-excluded</v>
+      </c>
+      <c r="D67" t="s">
+        <v>20</v>
+      </c>
+      <c r="E67" t="s">
+        <v>21</v>
+      </c>
+      <c r="F67" t="str">
+        <f t="shared" si="7"/>
+        <v>ILMN-DV-HG02145</v>
+      </c>
+      <c r="G67" t="b">
+        <v>0</v>
+      </c>
+      <c r="H67" t="b">
+        <v>1</v>
+      </c>
+      <c r="I67" t="s">
+        <v>33</v>
+      </c>
+      <c r="J67" t="str">
+        <f t="shared" si="8"/>
+        <v>GRCh38_HPRC-HG02145_dipz2k</v>
+      </c>
+      <c r="K67" t="s">
+        <v>24</v>
+      </c>
+      <c r="L67" t="s">
+        <v>25</v>
+      </c>
+      <c r="M67" t="s">
+        <v>26</v>
+      </c>
+      <c r="N67" t="s">
+        <v>27</v>
+      </c>
+      <c r="O67" t="str">
+        <f t="shared" si="9"/>
+        <v>HPRC-HG02145</v>
+      </c>
+      <c r="P67" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q67" t="s">
+        <v>30</v>
+      </c>
+      <c r="R67" t="s">
+        <v>31</v>
+      </c>
+      <c r="S67" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="68" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>65</v>
+      </c>
+      <c r="B68" t="str">
+        <f t="shared" si="5"/>
+        <v>GRCh38_T~HPRC-HG02148-dipz2k_Q~ILMNDV-HG02148</v>
+      </c>
+      <c r="C68" t="str">
+        <f t="shared" si="6"/>
+        <v>GRCh38_HPRC-HG02148-dipz2k_smvar-excluded</v>
+      </c>
+      <c r="D68" t="s">
+        <v>20</v>
+      </c>
+      <c r="E68" t="s">
+        <v>21</v>
+      </c>
+      <c r="F68" t="str">
+        <f t="shared" si="7"/>
+        <v>ILMN-DV-HG02148</v>
+      </c>
+      <c r="G68" t="b">
+        <v>0</v>
+      </c>
+      <c r="H68" t="b">
+        <v>1</v>
+      </c>
+      <c r="I68" t="s">
+        <v>33</v>
+      </c>
+      <c r="J68" t="str">
+        <f t="shared" si="8"/>
+        <v>GRCh38_HPRC-HG02148_dipz2k</v>
+      </c>
+      <c r="K68" t="s">
+        <v>24</v>
+      </c>
+      <c r="L68" t="s">
+        <v>25</v>
+      </c>
+      <c r="M68" t="s">
+        <v>26</v>
+      </c>
+      <c r="N68" t="s">
+        <v>27</v>
+      </c>
+      <c r="O68" t="str">
+        <f t="shared" si="9"/>
+        <v>HPRC-HG02148</v>
+      </c>
+      <c r="P68" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q68" t="s">
+        <v>30</v>
+      </c>
+      <c r="R68" t="s">
+        <v>31</v>
+      </c>
+      <c r="S68" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="69" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>66</v>
+      </c>
+      <c r="B69" t="str">
+        <f t="shared" si="5"/>
+        <v>GRCh38_T~HPRC-HG02257-dipz2k_Q~ILMNDV-HG02257</v>
+      </c>
+      <c r="C69" t="str">
+        <f t="shared" si="6"/>
+        <v>GRCh38_HPRC-HG02257-dipz2k_smvar-excluded</v>
+      </c>
+      <c r="D69" t="s">
+        <v>20</v>
+      </c>
+      <c r="E69" t="s">
+        <v>21</v>
+      </c>
+      <c r="F69" t="str">
+        <f t="shared" si="7"/>
+        <v>ILMN-DV-HG02257</v>
+      </c>
+      <c r="G69" t="b">
+        <v>0</v>
+      </c>
+      <c r="H69" t="b">
+        <v>1</v>
+      </c>
+      <c r="I69" t="s">
+        <v>33</v>
+      </c>
+      <c r="J69" t="str">
+        <f t="shared" si="8"/>
+        <v>GRCh38_HPRC-HG02257_dipz2k</v>
+      </c>
+      <c r="K69" t="s">
+        <v>24</v>
+      </c>
+      <c r="L69" t="s">
+        <v>25</v>
+      </c>
+      <c r="M69" t="s">
+        <v>26</v>
+      </c>
+      <c r="N69" t="s">
+        <v>27</v>
+      </c>
+      <c r="O69" t="str">
+        <f t="shared" si="9"/>
+        <v>HPRC-HG02257</v>
+      </c>
+      <c r="P69" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q69" t="s">
+        <v>30</v>
+      </c>
+      <c r="R69" t="s">
+        <v>31</v>
+      </c>
+      <c r="S69" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="70" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>69</v>
+      </c>
+      <c r="B70" t="str">
+        <f t="shared" si="5"/>
+        <v>GRCh38_T~HPRC-HG02572-dipz2k_Q~ILMNDV-HG02572</v>
+      </c>
+      <c r="C70" t="str">
+        <f t="shared" si="6"/>
+        <v>GRCh38_HPRC-HG02572-dipz2k_smvar-excluded</v>
+      </c>
+      <c r="D70" t="s">
+        <v>20</v>
+      </c>
+      <c r="E70" t="s">
+        <v>21</v>
+      </c>
+      <c r="F70" t="str">
+        <f t="shared" si="7"/>
+        <v>ILMN-DV-HG02572</v>
+      </c>
+      <c r="G70" t="b">
+        <v>0</v>
+      </c>
+      <c r="H70" t="b">
+        <v>1</v>
+      </c>
+      <c r="I70" t="s">
+        <v>33</v>
+      </c>
+      <c r="J70" t="str">
+        <f t="shared" si="8"/>
+        <v>GRCh38_HPRC-HG02572_dipz2k</v>
+      </c>
+      <c r="K70" t="s">
+        <v>24</v>
+      </c>
+      <c r="L70" t="s">
+        <v>25</v>
+      </c>
+      <c r="M70" t="s">
+        <v>26</v>
+      </c>
+      <c r="N70" t="s">
+        <v>27</v>
+      </c>
+      <c r="O70" t="str">
+        <f t="shared" si="9"/>
+        <v>HPRC-HG02572</v>
+      </c>
+      <c r="P70" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q70" t="s">
+        <v>30</v>
+      </c>
+      <c r="R70" t="s">
+        <v>31</v>
+      </c>
+      <c r="S70" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="71" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>70</v>
+      </c>
+      <c r="B71" t="str">
+        <f t="shared" si="5"/>
+        <v>GRCh38_T~HPRC-HG02622-dipz2k_Q~ILMNDV-HG02622</v>
+      </c>
+      <c r="C71" t="str">
+        <f t="shared" si="6"/>
+        <v>GRCh38_HPRC-HG02622-dipz2k_smvar-excluded</v>
+      </c>
+      <c r="D71" t="s">
+        <v>20</v>
+      </c>
+      <c r="E71" t="s">
+        <v>21</v>
+      </c>
+      <c r="F71" t="str">
+        <f t="shared" si="7"/>
+        <v>ILMN-DV-HG02622</v>
+      </c>
+      <c r="G71" t="b">
+        <v>0</v>
+      </c>
+      <c r="H71" t="b">
+        <v>1</v>
+      </c>
+      <c r="I71" t="s">
+        <v>33</v>
+      </c>
+      <c r="J71" t="str">
+        <f t="shared" si="8"/>
+        <v>GRCh38_HPRC-HG02622_dipz2k</v>
+      </c>
+      <c r="K71" t="s">
+        <v>24</v>
+      </c>
+      <c r="L71" t="s">
+        <v>25</v>
+      </c>
+      <c r="M71" t="s">
+        <v>26</v>
+      </c>
+      <c r="N71" t="s">
+        <v>27</v>
+      </c>
+      <c r="O71" t="str">
+        <f t="shared" si="9"/>
+        <v>HPRC-HG02622</v>
+      </c>
+      <c r="P71" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q71" t="s">
+        <v>30</v>
+      </c>
+      <c r="R71" t="s">
+        <v>31</v>
+      </c>
+      <c r="S71" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="72" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>71</v>
+      </c>
+      <c r="B72" t="str">
+        <f t="shared" si="5"/>
+        <v>GRCh38_T~HPRC-HG02630-dipz2k_Q~ILMNDV-HG02630</v>
+      </c>
+      <c r="C72" t="str">
+        <f t="shared" si="6"/>
+        <v>GRCh38_HPRC-HG02630-dipz2k_smvar-excluded</v>
+      </c>
+      <c r="D72" t="s">
+        <v>20</v>
+      </c>
+      <c r="E72" t="s">
+        <v>21</v>
+      </c>
+      <c r="F72" t="str">
+        <f t="shared" si="7"/>
+        <v>ILMN-DV-HG02630</v>
+      </c>
+      <c r="G72" t="b">
+        <v>0</v>
+      </c>
+      <c r="H72" t="b">
+        <v>1</v>
+      </c>
+      <c r="I72" t="s">
+        <v>33</v>
+      </c>
+      <c r="J72" t="str">
+        <f t="shared" si="8"/>
+        <v>GRCh38_HPRC-HG02630_dipz2k</v>
+      </c>
+      <c r="K72" t="s">
+        <v>24</v>
+      </c>
+      <c r="L72" t="s">
+        <v>25</v>
+      </c>
+      <c r="M72" t="s">
+        <v>26</v>
+      </c>
+      <c r="N72" t="s">
+        <v>27</v>
+      </c>
+      <c r="O72" t="str">
+        <f t="shared" si="9"/>
+        <v>HPRC-HG02630</v>
+      </c>
+      <c r="P72" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q72" t="s">
+        <v>30</v>
+      </c>
+      <c r="R72" t="s">
+        <v>31</v>
+      </c>
+      <c r="S72" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="73" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>72</v>
+      </c>
+      <c r="B73" t="str">
+        <f t="shared" si="5"/>
+        <v>GRCh38_T~HPRC-HG02717-dipz2k_Q~ILMNDV-HG02717</v>
+      </c>
+      <c r="C73" t="str">
+        <f t="shared" si="6"/>
+        <v>GRCh38_HPRC-HG02717-dipz2k_smvar-excluded</v>
+      </c>
+      <c r="D73" t="s">
+        <v>20</v>
+      </c>
+      <c r="E73" t="s">
+        <v>21</v>
+      </c>
+      <c r="F73" t="str">
+        <f t="shared" si="7"/>
+        <v>ILMN-DV-HG02717</v>
+      </c>
+      <c r="G73" t="b">
+        <v>0</v>
+      </c>
+      <c r="H73" t="b">
+        <v>1</v>
+      </c>
+      <c r="I73" t="s">
+        <v>33</v>
+      </c>
+      <c r="J73" t="str">
+        <f t="shared" si="8"/>
+        <v>GRCh38_HPRC-HG02717_dipz2k</v>
+      </c>
+      <c r="K73" t="s">
+        <v>24</v>
+      </c>
+      <c r="L73" t="s">
+        <v>25</v>
+      </c>
+      <c r="M73" t="s">
+        <v>26</v>
+      </c>
+      <c r="N73" t="s">
+        <v>27</v>
+      </c>
+      <c r="O73" t="str">
+        <f t="shared" si="9"/>
+        <v>HPRC-HG02717</v>
+      </c>
+      <c r="P73" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q73" t="s">
+        <v>30</v>
+      </c>
+      <c r="R73" t="s">
+        <v>31</v>
+      </c>
+      <c r="S73" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="74" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>41</v>
+      </c>
+      <c r="B74" t="str">
+        <f t="shared" si="5"/>
+        <v>GRCh38_T~HPRC-HG02723-dipz2k_Q~ILMNDV-HG02723</v>
+      </c>
+      <c r="C74" t="str">
+        <f t="shared" si="6"/>
+        <v>GRCh38_HPRC-HG02723-dipz2k_smvar-excluded</v>
+      </c>
+      <c r="D74" t="s">
+        <v>20</v>
+      </c>
+      <c r="E74" t="s">
+        <v>21</v>
+      </c>
+      <c r="F74" t="str">
+        <f t="shared" si="7"/>
+        <v>ILMN-DV-HG02723</v>
+      </c>
+      <c r="G74" t="b">
+        <v>0</v>
+      </c>
+      <c r="H74" t="b">
+        <v>1</v>
+      </c>
+      <c r="I74" t="s">
+        <v>33</v>
+      </c>
+      <c r="J74" t="str">
+        <f t="shared" si="8"/>
+        <v>GRCh38_HPRC-HG02723_dipz2k</v>
+      </c>
+      <c r="K74" t="s">
+        <v>24</v>
+      </c>
+      <c r="L74" t="s">
+        <v>25</v>
+      </c>
+      <c r="M74" t="s">
+        <v>26</v>
+      </c>
+      <c r="N74" t="s">
+        <v>27</v>
+      </c>
+      <c r="O74" t="str">
+        <f t="shared" si="9"/>
+        <v>HPRC-HG02723</v>
+      </c>
+      <c r="P74" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q74" t="s">
+        <v>30</v>
+      </c>
+      <c r="R74" t="s">
+        <v>31</v>
+      </c>
+      <c r="S74" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="75" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>42</v>
+      </c>
+      <c r="B75" t="str">
+        <f t="shared" si="5"/>
+        <v>GRCh38_T~HPRC-HG02818-dipz2k_Q~ILMNDV-HG02818</v>
+      </c>
+      <c r="C75" t="str">
+        <f t="shared" si="6"/>
+        <v>GRCh38_HPRC-HG02818-dipz2k_smvar-excluded</v>
+      </c>
+      <c r="D75" t="s">
+        <v>20</v>
+      </c>
+      <c r="E75" t="s">
+        <v>21</v>
+      </c>
+      <c r="F75" t="str">
+        <f t="shared" si="7"/>
+        <v>ILMN-DV-HG02818</v>
+      </c>
+      <c r="G75" t="b">
+        <v>0</v>
+      </c>
+      <c r="H75" t="b">
+        <v>1</v>
+      </c>
+      <c r="I75" t="s">
+        <v>33</v>
+      </c>
+      <c r="J75" t="str">
+        <f t="shared" si="8"/>
+        <v>GRCh38_HPRC-HG02818_dipz2k</v>
+      </c>
+      <c r="K75" t="s">
+        <v>24</v>
+      </c>
+      <c r="L75" t="s">
+        <v>25</v>
+      </c>
+      <c r="M75" t="s">
+        <v>26</v>
+      </c>
+      <c r="N75" t="s">
+        <v>27</v>
+      </c>
+      <c r="O75" t="str">
+        <f t="shared" si="9"/>
+        <v>HPRC-HG02818</v>
+      </c>
+      <c r="P75" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q75" t="s">
+        <v>30</v>
+      </c>
+      <c r="R75" t="s">
+        <v>31</v>
+      </c>
+      <c r="S75" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="76" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>73</v>
+      </c>
+      <c r="B76" t="str">
+        <f t="shared" si="5"/>
+        <v>GRCh38_T~HPRC-HG02886-dipz2k_Q~ILMNDV-HG02886</v>
+      </c>
+      <c r="C76" t="str">
+        <f t="shared" si="6"/>
+        <v>GRCh38_HPRC-HG02886-dipz2k_smvar-excluded</v>
+      </c>
+      <c r="D76" t="s">
+        <v>20</v>
+      </c>
+      <c r="E76" t="s">
+        <v>21</v>
+      </c>
+      <c r="F76" t="str">
+        <f t="shared" si="7"/>
+        <v>ILMN-DV-HG02886</v>
+      </c>
+      <c r="G76" t="b">
+        <v>0</v>
+      </c>
+      <c r="H76" t="b">
+        <v>1</v>
+      </c>
+      <c r="I76" t="s">
+        <v>33</v>
+      </c>
+      <c r="J76" t="str">
+        <f t="shared" si="8"/>
+        <v>GRCh38_HPRC-HG02886_dipz2k</v>
+      </c>
+      <c r="K76" t="s">
+        <v>24</v>
+      </c>
+      <c r="L76" t="s">
+        <v>25</v>
+      </c>
+      <c r="M76" t="s">
+        <v>26</v>
+      </c>
+      <c r="N76" t="s">
+        <v>27</v>
+      </c>
+      <c r="O76" t="str">
+        <f t="shared" si="9"/>
+        <v>HPRC-HG02886</v>
+      </c>
+      <c r="P76" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q76" t="s">
+        <v>30</v>
+      </c>
+      <c r="R76" t="s">
+        <v>31</v>
+      </c>
+      <c r="S76" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="77" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>43</v>
+      </c>
+      <c r="B77" t="str">
+        <f t="shared" si="5"/>
+        <v>GRCh38_T~HPRC-HG03098-dipz2k_Q~ILMNDV-HG03098</v>
+      </c>
+      <c r="C77" t="str">
+        <f t="shared" si="6"/>
+        <v>GRCh38_HPRC-HG03098-dipz2k_smvar-excluded</v>
+      </c>
+      <c r="D77" t="s">
+        <v>20</v>
+      </c>
+      <c r="E77" t="s">
+        <v>21</v>
+      </c>
+      <c r="F77" t="str">
+        <f t="shared" si="7"/>
+        <v>ILMN-DV-HG03098</v>
+      </c>
+      <c r="G77" t="b">
+        <v>0</v>
+      </c>
+      <c r="H77" t="b">
+        <v>1</v>
+      </c>
+      <c r="I77" t="s">
+        <v>33</v>
+      </c>
+      <c r="J77" t="str">
+        <f t="shared" si="8"/>
+        <v>GRCh38_HPRC-HG03098_dipz2k</v>
+      </c>
+      <c r="K77" t="s">
+        <v>24</v>
+      </c>
+      <c r="L77" t="s">
+        <v>25</v>
+      </c>
+      <c r="M77" t="s">
+        <v>26</v>
+      </c>
+      <c r="N77" t="s">
+        <v>27</v>
+      </c>
+      <c r="O77" t="str">
+        <f t="shared" si="9"/>
+        <v>HPRC-HG03098</v>
+      </c>
+      <c r="P77" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q77" t="s">
+        <v>30</v>
+      </c>
+      <c r="R77" t="s">
+        <v>31</v>
+      </c>
+      <c r="S77" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="78" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>74</v>
+      </c>
+      <c r="B78" t="str">
+        <f t="shared" si="5"/>
+        <v>GRCh38_T~HPRC-HG03453-dipz2k_Q~ILMNDV-HG03453</v>
+      </c>
+      <c r="C78" t="str">
+        <f t="shared" si="6"/>
+        <v>GRCh38_HPRC-HG03453-dipz2k_smvar-excluded</v>
+      </c>
+      <c r="D78" t="s">
+        <v>20</v>
+      </c>
+      <c r="E78" t="s">
+        <v>21</v>
+      </c>
+      <c r="F78" t="str">
+        <f t="shared" si="7"/>
+        <v>ILMN-DV-HG03453</v>
+      </c>
+      <c r="G78" t="b">
+        <v>0</v>
+      </c>
+      <c r="H78" t="b">
+        <v>1</v>
+      </c>
+      <c r="I78" t="s">
+        <v>33</v>
+      </c>
+      <c r="J78" t="str">
+        <f t="shared" si="8"/>
+        <v>GRCh38_HPRC-HG03453_dipz2k</v>
+      </c>
+      <c r="K78" t="s">
+        <v>24</v>
+      </c>
+      <c r="L78" t="s">
+        <v>25</v>
+      </c>
+      <c r="M78" t="s">
+        <v>26</v>
+      </c>
+      <c r="N78" t="s">
+        <v>27</v>
+      </c>
+      <c r="O78" t="str">
+        <f t="shared" si="9"/>
+        <v>HPRC-HG03453</v>
+      </c>
+      <c r="P78" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q78" t="s">
+        <v>30</v>
+      </c>
+      <c r="R78" t="s">
+        <v>31</v>
+      </c>
+      <c r="S78" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="79" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>44</v>
+      </c>
+      <c r="B79" t="str">
+        <f t="shared" si="5"/>
+        <v>GRCh38_T~HPRC-HG03486-dipz2k_Q~ILMNDV-HG03486</v>
+      </c>
+      <c r="C79" t="str">
+        <f t="shared" si="6"/>
+        <v>GRCh38_HPRC-HG03486-dipz2k_smvar-excluded</v>
+      </c>
+      <c r="D79" t="s">
+        <v>20</v>
+      </c>
+      <c r="E79" t="s">
+        <v>21</v>
+      </c>
+      <c r="F79" t="str">
+        <f t="shared" si="7"/>
+        <v>ILMN-DV-HG03486</v>
+      </c>
+      <c r="G79" t="b">
+        <v>0</v>
+      </c>
+      <c r="H79" t="b">
+        <v>1</v>
+      </c>
+      <c r="I79" t="s">
+        <v>33</v>
+      </c>
+      <c r="J79" t="str">
+        <f t="shared" si="8"/>
+        <v>GRCh38_HPRC-HG03486_dipz2k</v>
+      </c>
+      <c r="K79" t="s">
+        <v>24</v>
+      </c>
+      <c r="L79" t="s">
+        <v>25</v>
+      </c>
+      <c r="M79" t="s">
+        <v>26</v>
+      </c>
+      <c r="N79" t="s">
+        <v>27</v>
+      </c>
+      <c r="O79" t="str">
+        <f t="shared" si="9"/>
+        <v>HPRC-HG03486</v>
+      </c>
+      <c r="P79" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q79" t="s">
+        <v>30</v>
+      </c>
+      <c r="R79" t="s">
+        <v>31</v>
+      </c>
+      <c r="S79" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="80" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>45</v>
+      </c>
+      <c r="B80" t="str">
+        <f t="shared" si="5"/>
+        <v>GRCh38_T~HPRC-HG03492-dipz2k_Q~ILMNDV-HG03492</v>
+      </c>
+      <c r="C80" t="str">
+        <f t="shared" si="6"/>
+        <v>GRCh38_HPRC-HG03492-dipz2k_smvar-excluded</v>
+      </c>
+      <c r="D80" t="s">
+        <v>20</v>
+      </c>
+      <c r="E80" t="s">
+        <v>21</v>
+      </c>
+      <c r="F80" t="str">
+        <f t="shared" si="7"/>
+        <v>ILMN-DV-HG03492</v>
+      </c>
+      <c r="G80" t="b">
+        <v>0</v>
+      </c>
+      <c r="H80" t="b">
+        <v>1</v>
+      </c>
+      <c r="I80" t="s">
+        <v>33</v>
+      </c>
+      <c r="J80" t="str">
+        <f t="shared" si="8"/>
+        <v>GRCh38_HPRC-HG03492_dipz2k</v>
+      </c>
+      <c r="K80" t="s">
+        <v>24</v>
+      </c>
+      <c r="L80" t="s">
+        <v>25</v>
+      </c>
+      <c r="M80" t="s">
+        <v>26</v>
+      </c>
+      <c r="N80" t="s">
+        <v>27</v>
+      </c>
+      <c r="O80" t="str">
+        <f t="shared" si="9"/>
+        <v>HPRC-HG03492</v>
+      </c>
+      <c r="P80" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q80" t="s">
+        <v>30</v>
+      </c>
+      <c r="R80" t="s">
+        <v>31</v>
+      </c>
+      <c r="S80" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="81" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>75</v>
+      </c>
+      <c r="B81" t="str">
+        <f t="shared" si="5"/>
+        <v>GRCh38_T~HPRC-HG03516-dipz2k_Q~ILMNDV-HG03516</v>
+      </c>
+      <c r="C81" t="str">
+        <f t="shared" si="6"/>
+        <v>GRCh38_HPRC-HG03516-dipz2k_smvar-excluded</v>
+      </c>
+      <c r="D81" t="s">
+        <v>20</v>
+      </c>
+      <c r="E81" t="s">
+        <v>21</v>
+      </c>
+      <c r="F81" t="str">
+        <f t="shared" si="7"/>
+        <v>ILMN-DV-HG03516</v>
+      </c>
+      <c r="G81" t="b">
+        <v>0</v>
+      </c>
+      <c r="H81" t="b">
+        <v>1</v>
+      </c>
+      <c r="I81" t="s">
+        <v>33</v>
+      </c>
+      <c r="J81" t="str">
+        <f t="shared" si="8"/>
+        <v>GRCh38_HPRC-HG03516_dipz2k</v>
+      </c>
+      <c r="K81" t="s">
+        <v>24</v>
+      </c>
+      <c r="L81" t="s">
+        <v>25</v>
+      </c>
+      <c r="M81" t="s">
+        <v>26</v>
+      </c>
+      <c r="N81" t="s">
+        <v>27</v>
+      </c>
+      <c r="O81" t="str">
+        <f t="shared" si="9"/>
+        <v>HPRC-HG03516</v>
+      </c>
+      <c r="P81" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q81" t="s">
+        <v>30</v>
+      </c>
+      <c r="R81" t="s">
+        <v>31</v>
+      </c>
+      <c r="S81" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="82" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>76</v>
+      </c>
+      <c r="B82" t="str">
+        <f t="shared" si="5"/>
+        <v>GRCh38_T~HPRC-HG03540-dipz2k_Q~ILMNDV-HG03540</v>
+      </c>
+      <c r="C82" t="str">
+        <f t="shared" si="6"/>
+        <v>GRCh38_HPRC-HG03540-dipz2k_smvar-excluded</v>
+      </c>
+      <c r="D82" t="s">
+        <v>20</v>
+      </c>
+      <c r="E82" t="s">
+        <v>21</v>
+      </c>
+      <c r="F82" t="str">
+        <f t="shared" si="7"/>
+        <v>ILMN-DV-HG03540</v>
+      </c>
+      <c r="G82" t="b">
+        <v>0</v>
+      </c>
+      <c r="H82" t="b">
+        <v>1</v>
+      </c>
+      <c r="I82" t="s">
+        <v>33</v>
+      </c>
+      <c r="J82" t="str">
+        <f t="shared" si="8"/>
+        <v>GRCh38_HPRC-HG03540_dipz2k</v>
+      </c>
+      <c r="K82" t="s">
+        <v>24</v>
+      </c>
+      <c r="L82" t="s">
+        <v>25</v>
+      </c>
+      <c r="M82" t="s">
+        <v>26</v>
+      </c>
+      <c r="N82" t="s">
+        <v>27</v>
+      </c>
+      <c r="O82" t="str">
+        <f t="shared" si="9"/>
+        <v>HPRC-HG03540</v>
+      </c>
+      <c r="P82" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q82" t="s">
+        <v>30</v>
+      </c>
+      <c r="R82" t="s">
+        <v>31</v>
+      </c>
+      <c r="S82" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="83" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>77</v>
+      </c>
+      <c r="B83" t="str">
+        <f t="shared" si="5"/>
+        <v>GRCh38_T~HPRC-HG03579-dipz2k_Q~ILMNDV-HG03579</v>
+      </c>
+      <c r="C83" t="str">
+        <f t="shared" si="6"/>
+        <v>GRCh38_HPRC-HG03579-dipz2k_smvar-excluded</v>
+      </c>
+      <c r="D83" t="s">
+        <v>20</v>
+      </c>
+      <c r="E83" t="s">
+        <v>21</v>
+      </c>
+      <c r="F83" t="str">
+        <f t="shared" si="7"/>
+        <v>ILMN-DV-HG03579</v>
+      </c>
+      <c r="G83" t="b">
+        <v>0</v>
+      </c>
+      <c r="H83" t="b">
+        <v>1</v>
+      </c>
+      <c r="I83" t="s">
+        <v>33</v>
+      </c>
+      <c r="J83" t="str">
+        <f t="shared" si="8"/>
+        <v>GRCh38_HPRC-HG03579_dipz2k</v>
+      </c>
+      <c r="K83" t="s">
+        <v>24</v>
+      </c>
+      <c r="L83" t="s">
+        <v>25</v>
+      </c>
+      <c r="M83" t="s">
+        <v>26</v>
+      </c>
+      <c r="N83" t="s">
+        <v>27</v>
+      </c>
+      <c r="O83" t="str">
+        <f t="shared" si="9"/>
+        <v>HPRC-HG03579</v>
+      </c>
+      <c r="P83" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q83" t="s">
+        <v>30</v>
+      </c>
+      <c r="R83" t="s">
+        <v>31</v>
+      </c>
+      <c r="S83" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="84" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>46</v>
+      </c>
+      <c r="B84" t="str">
+        <f t="shared" si="5"/>
+        <v>GRCh38_T~HPRC-NA18906-dipz2k_Q~ILMNDV-NA18906</v>
+      </c>
+      <c r="C84" t="str">
+        <f t="shared" si="6"/>
+        <v>GRCh38_HPRC-NA18906-dipz2k_smvar-excluded</v>
+      </c>
+      <c r="D84" t="s">
+        <v>20</v>
+      </c>
+      <c r="E84" t="s">
+        <v>21</v>
+      </c>
+      <c r="F84" t="str">
+        <f t="shared" si="7"/>
+        <v>ILMN-DV-NA18906</v>
+      </c>
+      <c r="G84" t="b">
+        <v>0</v>
+      </c>
+      <c r="H84" t="b">
+        <v>1</v>
+      </c>
+      <c r="I84" t="s">
+        <v>33</v>
+      </c>
+      <c r="J84" t="str">
+        <f t="shared" si="8"/>
+        <v>GRCh38_HPRC-NA18906_dipz2k</v>
+      </c>
+      <c r="K84" t="s">
+        <v>24</v>
+      </c>
+      <c r="L84" t="s">
+        <v>25</v>
+      </c>
+      <c r="M84" t="s">
+        <v>26</v>
+      </c>
+      <c r="N84" t="s">
+        <v>27</v>
+      </c>
+      <c r="O84" t="str">
+        <f t="shared" si="9"/>
+        <v>HPRC-NA18906</v>
+      </c>
+      <c r="P84" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q84" t="s">
+        <v>30</v>
+      </c>
+      <c r="R84" t="s">
+        <v>31</v>
+      </c>
+      <c r="S84" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>